<commit_message>
Modify binomial lattice model
</commit_message>
<xml_diff>
--- a/data/correlation/ship_demand_month.xlsx
+++ b/data/correlation/ship_demand_month.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C15BE7B-4A64-FE40-AD5E-CCF5811005C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25762C-6C04-6049-BAF8-1F0961D7122B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="1" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
   </bookViews>
   <sheets>
     <sheet name="海事センター" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="77">
   <si>
     <t>Gap</t>
     <phoneticPr fontId="1"/>
@@ -444,6 +444,16 @@
     <t>平均</t>
     <rPh sb="0" eb="2">
       <t>ヘイキn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一隻あたりの需要</t>
+    <rPh sb="0" eb="2">
+      <t>イッセ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジュヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5879,8 +5889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35A8DBA-102A-6246-87AB-BC7138704158}">
   <dimension ref="A1:Y216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="D211" sqref="D211"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -5900,7 +5910,7 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>52</v>
@@ -9838,7 +9848,7 @@
         <v>5119</v>
       </c>
       <c r="D195">
-        <f t="shared" ref="D195:D205" si="3">B195/C195</f>
+        <f t="shared" ref="D195:D204" si="3">B195/C195</f>
         <v>2.1851454206550758E-3</v>
       </c>
       <c r="E195">
@@ -10123,8 +10133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1EF3A6-C6D7-6C40-A397-3F20CE72D830}">
   <dimension ref="A1:T216"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -10359,9 +10369,7 @@
       <c r="J11">
         <v>1.9688028474345903E-3</v>
       </c>
-      <c r="K11" s="8">
-        <v>830</v>
-      </c>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1">
@@ -10380,9 +10388,7 @@
       <c r="J12">
         <v>1.97622375637105E-3</v>
       </c>
-      <c r="K12" s="8">
-        <v>850</v>
-      </c>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="21" thickBot="1">
       <c r="A13" s="1">
@@ -10403,9 +10409,7 @@
       <c r="J13">
         <v>1.9910655742439685E-3</v>
       </c>
-      <c r="K13" s="8">
-        <v>750</v>
-      </c>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1">
@@ -10427,9 +10431,7 @@
       <c r="J14">
         <v>2.0021969384981311E-3</v>
       </c>
-      <c r="K14" s="8">
-        <v>740</v>
-      </c>
+      <c r="K14" s="8"/>
       <c r="L14" t="s">
         <v>1</v>
       </c>
@@ -10451,9 +10453,7 @@
       <c r="J15">
         <v>1.9459999522020042E-3</v>
       </c>
-      <c r="K15" s="8">
-        <v>670</v>
-      </c>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:13" ht="21" thickBot="1">
       <c r="A16" s="1">
@@ -10466,7 +10466,7 @@
         <v>27</v>
       </c>
       <c r="H16" s="4">
-        <v>-0.3974754619546822</v>
+        <v>-0.42567296035021712</v>
       </c>
       <c r="I16" s="4">
         <v>1</v>
@@ -10474,9 +10474,7 @@
       <c r="J16">
         <v>1.9531992319356539E-3</v>
       </c>
-      <c r="K16" s="8">
-        <v>680</v>
-      </c>
+      <c r="K16" s="8"/>
       <c r="L16" s="6" t="s">
         <v>2</v>
       </c>
@@ -10503,13 +10501,13 @@
         <v>1.9531992319356539E-3</v>
       </c>
       <c r="K17" s="8">
-        <v>870</v>
+        <v>830</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M17" s="3">
-        <v>0.39747546195468192</v>
+        <v>0.42567296035021773</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -10530,13 +10528,13 @@
         <v>1.9603985116693041E-3</v>
       </c>
       <c r="K18" s="8">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M18" s="3">
-        <v>0.1579867428560878</v>
+        <v>0.18119746917331805</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="21" thickBot="1">
@@ -10559,13 +10557,13 @@
         <v>1.9603985116693041E-3</v>
       </c>
       <c r="K19" s="8">
-        <v>820</v>
+        <v>750</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="M19" s="3">
-        <v>0.14595798203974619</v>
+        <v>0.16915625548469038</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -10589,13 +10587,13 @@
         <v>1.9675977914029538E-3</v>
       </c>
       <c r="K20" s="8">
-        <v>690</v>
+        <v>740</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="M20" s="3">
-        <v>151.11672840728676</v>
+        <v>149.82341076275492</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="21" thickBot="1">
@@ -10616,13 +10614,13 @@
         <v>1.9675977914029538E-3</v>
       </c>
       <c r="K21" s="8">
-        <v>750</v>
+        <v>670</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M21" s="4">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="21" thickBot="1">
@@ -10645,7 +10643,7 @@
         <v>1.9747970711366035E-3</v>
       </c>
       <c r="K22" s="8">
-        <v>820</v>
+        <v>680</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="21" thickBot="1">
@@ -10669,7 +10667,7 @@
         <v>1.9747970711366035E-3</v>
       </c>
       <c r="K23" s="8">
-        <v>730</v>
+        <v>870</v>
       </c>
       <c r="L23" t="s">
         <v>8</v>
@@ -10693,7 +10691,7 @@
         <v>1.9783967101793245E-3</v>
       </c>
       <c r="K24" s="8">
-        <v>650</v>
+        <v>800</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
@@ -10732,7 +10730,7 @@
         <v>1.9819963508702532E-3</v>
       </c>
       <c r="K25" s="8">
-        <v>850</v>
+        <v>820</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>9</v>
@@ -10741,16 +10739,16 @@
         <v>1</v>
       </c>
       <c r="N25" s="3">
-        <v>299933.40768348263</v>
+        <v>337785.67137277918</v>
       </c>
       <c r="O25" s="3">
-        <v>299933.40768348263</v>
+        <v>337785.67137277918</v>
       </c>
       <c r="P25" s="3">
-        <v>13.134082992277628</v>
+        <v>15.048106765553877</v>
       </c>
       <c r="Q25" s="3">
-        <v>5.4567444789463491E-4</v>
+        <v>2.390576318615182E-4</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -10774,19 +10772,19 @@
         <v>1.9855959899129747E-3</v>
       </c>
       <c r="K26" s="8">
-        <v>900</v>
+        <v>690</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M26" s="3">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N26" s="3">
-        <v>1598538.5923165167</v>
+        <v>1526399.7000557929</v>
       </c>
       <c r="O26" s="3">
-        <v>22836.265604521668</v>
+        <v>22447.054412585188</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -10809,16 +10807,16 @@
         <v>1.9876231439393938E-3</v>
       </c>
       <c r="K27" s="8">
-        <v>108</v>
+        <v>750</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M27" s="4">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N27" s="4">
-        <v>1898471.9999999993</v>
+        <v>1864185.3714285721</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -10844,7 +10842,7 @@
         <v>1.9876231439393938E-3</v>
       </c>
       <c r="K28" s="8">
-        <v>1180</v>
+        <v>820</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -10868,7 +10866,7 @@
         <v>1.9948167325428193E-3</v>
       </c>
       <c r="K29" s="8">
-        <v>1160</v>
+        <v>730</v>
       </c>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
@@ -10914,34 +10912,34 @@
         <v>1.9948167325428193E-3</v>
       </c>
       <c r="K30" s="8">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M30" s="3">
-        <v>2578.5020445985056</v>
+        <v>2515.3706917308596</v>
       </c>
       <c r="N30" s="3">
-        <v>495.01889941830285</v>
+        <v>445.32782754835785</v>
       </c>
       <c r="O30" s="3">
-        <v>5.2088961605880213</v>
+        <v>5.6483573137088925</v>
       </c>
       <c r="P30" s="3">
-        <v>1.8240491704180346E-6</v>
+        <v>3.4600806550774843E-7</v>
       </c>
       <c r="Q30" s="3">
-        <v>1591.2179805705146</v>
+        <v>1626.7328475569648</v>
       </c>
       <c r="R30" s="3">
-        <v>3565.7861086264966</v>
+        <v>3404.0085359047544</v>
       </c>
       <c r="S30" s="3">
-        <v>1591.2179805705146</v>
+        <v>1626.7328475569648</v>
       </c>
       <c r="T30" s="3">
-        <v>3565.7861086264966</v>
+        <v>3404.0085359047544</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="21" thickBot="1">
@@ -10964,34 +10962,34 @@
         <v>2.0020103211462453E-3</v>
       </c>
       <c r="K31" s="8">
-        <v>1010</v>
+        <v>850</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M31" s="4">
-        <v>-869948.03845961706</v>
+        <v>-829816.26459999999</v>
       </c>
       <c r="N31" s="4">
-        <v>240045.42604950501</v>
+        <v>213914.88770037598</v>
       </c>
       <c r="O31" s="4">
-        <v>-3.624097541771973</v>
+        <v>-3.8791889314074202</v>
       </c>
       <c r="P31" s="4">
-        <v>5.456744478946297E-4</v>
+        <v>2.3905763186152188E-4</v>
       </c>
       <c r="Q31" s="4">
-        <v>-1348703.5446836755</v>
+        <v>-1256676.7770069637</v>
       </c>
       <c r="R31" s="4">
-        <v>-391192.53223555861</v>
+        <v>-402955.75225415581</v>
       </c>
       <c r="S31" s="4">
-        <v>-1348703.5446836755</v>
+        <v>-1256676.7770069637</v>
       </c>
       <c r="T31" s="4">
-        <v>-391192.53223555861</v>
+        <v>-402955.75225415581</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -11015,7 +11013,7 @@
         <v>2.0020103211462453E-3</v>
       </c>
       <c r="K32" s="8">
-        <v>1090</v>
+        <v>900</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -11036,7 +11034,7 @@
         <v>2.0092039097496708E-3</v>
       </c>
       <c r="K33" s="8">
-        <v>1040</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" thickBot="1">
@@ -11059,7 +11057,7 @@
         <v>2.0092039097496708E-3</v>
       </c>
       <c r="K34" s="8">
-        <v>1080</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -11083,7 +11081,7 @@
         <v>2.0163974983530963E-3</v>
       </c>
       <c r="K35" s="8">
-        <v>970</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -11104,7 +11102,7 @@
         <v>2.0163974983530963E-3</v>
       </c>
       <c r="K36" s="8">
-        <v>950</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="21" thickBot="1">
@@ -11127,7 +11125,7 @@
         <v>2.0235910869565213E-3</v>
       </c>
       <c r="K37" s="8">
-        <v>910</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -11141,7 +11139,7 @@
         <v>2.0235910869565213E-3</v>
       </c>
       <c r="K38" s="8">
-        <v>920</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -11155,7 +11153,7 @@
         <v>2.0219933999081727E-3</v>
       </c>
       <c r="K39" s="8">
-        <v>800</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -11169,7 +11167,7 @@
         <v>2.0291558474353926E-3</v>
       </c>
       <c r="K40" s="8">
-        <v>820</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -11183,7 +11181,7 @@
         <v>2.0327370703791159E-3</v>
       </c>
       <c r="K41" s="8">
-        <v>830</v>
+        <v>970</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -11197,7 +11195,7 @@
         <v>2.0434807424898334E-3</v>
       </c>
       <c r="K42" s="8">
-        <v>850</v>
+        <v>950</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -11211,7 +11209,7 @@
         <v>2.0506431900170537E-3</v>
       </c>
       <c r="K43" s="8">
-        <v>860</v>
+        <v>910</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -11225,7 +11223,7 @@
         <v>2.0506431900170537E-3</v>
       </c>
       <c r="K44" s="8">
-        <v>820</v>
+        <v>920</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -11253,7 +11251,7 @@
         <v>2.064968085071494E-3</v>
       </c>
       <c r="K46" s="8">
-        <v>800</v>
+        <v>820</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -11267,7 +11265,7 @@
         <v>2.0721305309589402E-3</v>
       </c>
       <c r="K47" s="8">
-        <v>820</v>
+        <v>830</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -11281,7 +11279,7 @@
         <v>2.0792929784861605E-3</v>
       </c>
       <c r="K48" s="8">
-        <v>820</v>
+        <v>850</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -11295,7 +11293,7 @@
         <v>2.0864554260133805E-3</v>
       </c>
       <c r="K49" s="8">
-        <v>890</v>
+        <v>860</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -11316,7 +11314,7 @@
         <v>2.0936178735406008E-3</v>
       </c>
       <c r="K50" s="8">
-        <v>850</v>
+        <v>820</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -11337,7 +11335,7 @@
         <v>2.0921351345613692E-3</v>
       </c>
       <c r="K51" s="8">
-        <v>860</v>
+        <v>800</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -11358,7 +11356,7 @@
         <v>2.0921351345613692E-3</v>
       </c>
       <c r="K52" s="8">
-        <v>850</v>
+        <v>800</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -11379,7 +11377,7 @@
         <v>2.0957016215951397E-3</v>
       </c>
       <c r="K53" s="8">
-        <v>840</v>
+        <v>820</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -11400,7 +11398,7 @@
         <v>2.0992681069958849E-3</v>
       </c>
       <c r="K54" s="8">
-        <v>840</v>
+        <v>820</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -11421,7 +11419,7 @@
         <v>2.0992681069958849E-3</v>
       </c>
       <c r="K55" s="8">
-        <v>810</v>
+        <v>890</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -11484,7 +11482,7 @@
         <v>2.1064010794304001E-3</v>
       </c>
       <c r="K58" s="8">
-        <v>810</v>
+        <v>850</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -11505,7 +11503,7 @@
         <v>2.1064010794304001E-3</v>
       </c>
       <c r="K59" s="8">
-        <v>790</v>
+        <v>840</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -11526,7 +11524,7 @@
         <v>2.1099675664641715E-3</v>
       </c>
       <c r="K60" s="8">
-        <v>700</v>
+        <v>840</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -11547,7 +11545,7 @@
         <v>2.1135340518649163E-3</v>
       </c>
       <c r="K61" s="8">
-        <v>830</v>
+        <v>810</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -11568,7 +11566,7 @@
         <v>2.1135340518649163E-3</v>
       </c>
       <c r="K62" s="8">
-        <v>780</v>
+        <v>850</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -11589,7 +11587,7 @@
         <v>2.0685393683672164E-3</v>
       </c>
       <c r="K63" s="8">
-        <v>770</v>
+        <v>860</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -11610,7 +11608,7 @@
         <v>2.0755204881089374E-3</v>
       </c>
       <c r="K64" s="8">
-        <v>710</v>
+        <v>810</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -11631,7 +11629,7 @@
         <v>2.0825016078506588E-3</v>
       </c>
       <c r="K65" s="8">
-        <v>680</v>
+        <v>790</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -11652,7 +11650,7 @@
         <v>2.0894827275923793E-3</v>
       </c>
       <c r="K66" s="8">
-        <v>640</v>
+        <v>700</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -11673,7 +11671,7 @@
         <v>2.0894827275923793E-3</v>
       </c>
       <c r="K67" s="8">
-        <v>660</v>
+        <v>830</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -11694,7 +11692,7 @@
         <v>2.0964638473341003E-3</v>
       </c>
       <c r="K68" s="8">
-        <v>640</v>
+        <v>780</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -11715,7 +11713,7 @@
         <v>2.1034449670758217E-3</v>
       </c>
       <c r="K69" s="8">
-        <v>650</v>
+        <v>770</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -11736,7 +11734,7 @@
         <v>2.1104260868175426E-3</v>
       </c>
       <c r="K70" s="8">
-        <v>610</v>
+        <v>710</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -11757,7 +11755,7 @@
         <v>2.1104260868175426E-3</v>
       </c>
       <c r="K71" s="8">
-        <v>640</v>
+        <v>680</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -11778,7 +11776,7 @@
         <v>2.1174072065592636E-3</v>
       </c>
       <c r="K72" s="8">
-        <v>660</v>
+        <v>640</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -11799,7 +11797,7 @@
         <v>2.1243883263009846E-3</v>
       </c>
       <c r="K73" s="8">
-        <v>650</v>
+        <v>660</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -11820,7 +11818,7 @@
         <v>2.1243883263009846E-3</v>
       </c>
       <c r="K74" s="8">
-        <v>630</v>
+        <v>640</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -11841,7 +11839,7 @@
         <v>2.1709240655727029E-3</v>
       </c>
       <c r="K75" s="8">
-        <v>580</v>
+        <v>650</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -11862,7 +11860,7 @@
         <v>2.1851454206550758E-3</v>
       </c>
       <c r="K76" s="8">
-        <v>570</v>
+        <v>610</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -11883,7 +11881,7 @@
         <v>2.1922560981962624E-3</v>
       </c>
       <c r="K77" s="8">
-        <v>610</v>
+        <v>640</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -11904,7 +11902,7 @@
         <v>2.2029221136940806E-3</v>
       </c>
       <c r="K78" s="8">
-        <v>600</v>
+        <v>660</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -11925,7 +11923,7 @@
         <v>2.2135881308198214E-3</v>
       </c>
       <c r="K79" s="8">
-        <v>580</v>
+        <v>650</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -11946,7 +11944,7 @@
         <v>2.220698808361008E-3</v>
       </c>
       <c r="K80" s="8">
-        <v>620</v>
+        <v>630</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -11967,7 +11965,7 @@
         <v>2.2349201634433808E-3</v>
       </c>
       <c r="K81" s="8">
-        <v>630</v>
+        <v>580</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -11988,7 +11986,7 @@
         <v>2.2420308409845675E-3</v>
       </c>
       <c r="K82" s="8">
-        <v>690</v>
+        <v>570</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -12008,6 +12006,9 @@
       <c r="J83">
         <v>2.2491415185257537E-3</v>
       </c>
+      <c r="K83" s="8">
+        <v>610</v>
+      </c>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="1">
@@ -12026,6 +12027,9 @@
       <c r="J84">
         <v>2.2633628736081269E-3</v>
       </c>
+      <c r="K84" s="8">
+        <v>600</v>
+      </c>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="1">
@@ -12044,6 +12048,9 @@
       <c r="J85">
         <v>2.2704735511493127E-3</v>
       </c>
+      <c r="K85" s="8">
+        <v>580</v>
+      </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="1">
@@ -12062,6 +12069,9 @@
       <c r="J86">
         <v>2.2811395666471317E-3</v>
       </c>
+      <c r="K86" s="8">
+        <v>620</v>
+      </c>
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="1">
@@ -12077,6 +12087,9 @@
         <f t="shared" si="0"/>
         <v>1.9904697246107368E-3</v>
       </c>
+      <c r="K87" s="8">
+        <v>630</v>
+      </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="1">
@@ -12091,6 +12104,9 @@
       <c r="D88">
         <f t="shared" si="0"/>
         <v>1.9989288364706797E-3</v>
+      </c>
+      <c r="K88" s="8">
+        <v>690</v>
       </c>
     </row>
     <row r="89" spans="1:11">

</xml_diff>

<commit_message>
change the way of generating ship market
</commit_message>
<xml_diff>
--- a/data/correlation/ship_demand_month.xlsx
+++ b/data/correlation/ship_demand_month.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9996B8-5AEC-954E-9018-D23A84F5D822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9025E32-2B38-8C41-A5CF-217172A097C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
+    <workbookView xWindow="9760" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
   </bookViews>
   <sheets>
     <sheet name="海事センター" sheetId="5" r:id="rId1"/>
@@ -21,12 +21,6 @@
     <sheet name="行き" sheetId="6" r:id="rId6"/>
     <sheet name="帰り" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'帰り（コンテナ積載数）'!$I$1:$I$72</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'帰り（コンテナ積載数）'!$J$1:$J$72</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'帰り（コンテナ積載数）'!$I$1:$I$72</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'帰り（コンテナ積載数）'!$J$1:$J$72</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -8598,7 +8592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35A8DBA-102A-6246-87AB-BC7138704158}">
   <dimension ref="A1:Y216"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A119" workbookViewId="0">
       <selection sqref="A1:E204"/>
     </sheetView>
   </sheetViews>
@@ -13033,8 +13027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40FD581-74FB-F94A-9780-764D633DA0D6}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="107" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="107" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -14440,7 +14434,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <f>($C$73-$C$61)*D61/12+$C$61</f>
+        <f t="shared" ref="E61:E72" si="1">($C$73-$C$61)*D61/12+$C$61</f>
         <v>7239</v>
       </c>
       <c r="F61">
@@ -14469,11 +14463,11 @@
         <v>1</v>
       </c>
       <c r="E62">
-        <f>($C$73-$C$61)*D62/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7317.25</v>
       </c>
       <c r="F62">
-        <f t="shared" ref="F62:F125" si="1">B62/E62</f>
+        <f t="shared" ref="F62:F125" si="2">B62/E62</f>
         <v>9.5910485621875249E-4</v>
       </c>
       <c r="G62">
@@ -14498,11 +14492,11 @@
         <v>2</v>
       </c>
       <c r="E63">
-        <f>($C$73-$C$61)*D63/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7395.5</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5633957767110632E-4</v>
       </c>
       <c r="G63">
@@ -14527,11 +14521,11 @@
         <v>3</v>
       </c>
       <c r="E64">
-        <f>($C$73-$C$61)*D64/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7473.75</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5606736410771035E-4</v>
       </c>
       <c r="G64">
@@ -14556,11 +14550,11 @@
         <v>4</v>
       </c>
       <c r="E65">
-        <f>($C$73-$C$61)*D65/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7552</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4857100657662428E-4</v>
       </c>
       <c r="G65">
@@ -14585,15 +14579,15 @@
         <v>5</v>
       </c>
       <c r="E66">
-        <f>($C$73-$C$61)*D66/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7630.25</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4599883075041234E-4</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66:G72" si="2">1000*H66</f>
+        <f t="shared" ref="G66:G72" si="3">1000*H66</f>
         <v>0.57191529004525643</v>
       </c>
       <c r="H66">
@@ -14614,15 +14608,15 @@
         <v>6</v>
       </c>
       <c r="E67">
-        <f>($C$73-$C$61)*D67/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7708.5</v>
       </c>
       <c r="F67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4347887602430213E-4</v>
       </c>
       <c r="G67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.57316422857142868</v>
       </c>
       <c r="H67">
@@ -14643,15 +14637,15 @@
         <v>7</v>
       </c>
       <c r="E68">
-        <f>($C$73-$C$61)*D68/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7786.75</v>
       </c>
       <c r="F68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3867229256964298E-4</v>
       </c>
       <c r="G68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.57624400110810758</v>
       </c>
       <c r="H68">
@@ -14672,15 +14666,15 @@
         <v>8</v>
       </c>
       <c r="E69">
-        <f>($C$73-$C$61)*D69/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7865</v>
       </c>
       <c r="F69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3627537327823686E-4</v>
       </c>
       <c r="G69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.57748595526818958</v>
       </c>
       <c r="H69">
@@ -14701,15 +14695,15 @@
         <v>9</v>
       </c>
       <c r="E70">
-        <f>($C$73-$C$61)*D70/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7943.25</v>
       </c>
       <c r="F70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3163445304713646E-4</v>
       </c>
       <c r="G70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.57872537070857699</v>
       </c>
       <c r="H70">
@@ -14730,15 +14724,15 @@
         <v>10</v>
       </c>
       <c r="E71">
-        <f>($C$73-$C$61)*D71/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>8021.5</v>
       </c>
       <c r="F71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2708407737538702E-4</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.581790031634976</v>
       </c>
       <c r="H71">
@@ -14759,15 +14753,15 @@
         <v>11</v>
       </c>
       <c r="E72">
-        <f>($C$73-$C$61)*D72/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>8099.75</v>
       </c>
       <c r="F72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2486857793964831E-4</v>
       </c>
       <c r="G72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.58302252863472948</v>
       </c>
       <c r="H72">
@@ -14795,7 +14789,7 @@
         <v>8178</v>
       </c>
       <c r="F73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2492093176815848E-4</v>
       </c>
       <c r="G73">
@@ -14814,11 +14808,11 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <f t="shared" ref="E74:E84" si="3">($C$85-$C$73)*D74/12+$C$73</f>
+        <f t="shared" ref="E74:E84" si="4">($C$85-$C$73)*D74/12+$C$73</f>
         <v>8289.75</v>
       </c>
       <c r="F74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1464798807764616E-4</v>
       </c>
     </row>
@@ -14833,11 +14827,11 @@
         <v>2</v>
       </c>
       <c r="E75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8401.5</v>
       </c>
       <c r="F75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1331334335138564E-4</v>
       </c>
     </row>
@@ -14852,11 +14846,11 @@
         <v>3</v>
       </c>
       <c r="E76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8513.25</v>
       </c>
       <c r="F76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0560028338178711E-4</v>
       </c>
     </row>
@@ -14871,11 +14865,11 @@
         <v>4</v>
       </c>
       <c r="E77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8625</v>
       </c>
       <c r="F77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0019721159420292E-4</v>
       </c>
     </row>
@@ -14890,7 +14884,7 @@
         <v>5</v>
       </c>
       <c r="E78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8736.75</v>
       </c>
       <c r="F78">
@@ -14909,11 +14903,11 @@
         <v>6</v>
       </c>
       <c r="E79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8848.5</v>
       </c>
       <c r="F79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0831187602418491E-4</v>
       </c>
     </row>
@@ -14928,11 +14922,11 @@
         <v>7</v>
       </c>
       <c r="E80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8960.25</v>
       </c>
       <c r="F80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.051083118030562E-4</v>
       </c>
     </row>
@@ -14947,11 +14941,11 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9072</v>
       </c>
       <c r="F81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0198367146164017E-4</v>
       </c>
     </row>
@@ -14966,11 +14960,11 @@
         <v>9</v>
       </c>
       <c r="E82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9183.75</v>
       </c>
       <c r="F82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9695333650923284E-4</v>
       </c>
     </row>
@@ -14985,11 +14979,11 @@
         <v>10</v>
       </c>
       <c r="E83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9295.5</v>
       </c>
       <c r="F83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9400186335682153E-4</v>
       </c>
     </row>
@@ -15004,11 +14998,11 @@
         <v>11</v>
       </c>
       <c r="E84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9407.25</v>
       </c>
       <c r="F84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9112051166210474E-4</v>
       </c>
     </row>
@@ -15030,7 +15024,7 @@
         <v>9519</v>
       </c>
       <c r="F85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8448292800364194E-4</v>
       </c>
     </row>
@@ -15045,11 +15039,11 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <f t="shared" ref="E86:E96" si="4">($C$97-$C$85)*D86/12+$C$85</f>
+        <f t="shared" ref="E86:E95" si="5">($C$97-$C$85)*D86/12+$C$85</f>
         <v>9627.5</v>
       </c>
       <c r="F86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8207656279754173E-4</v>
       </c>
     </row>
@@ -15064,11 +15058,11 @@
         <v>2</v>
       </c>
       <c r="E87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9736</v>
       </c>
       <c r="F87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.759851752944399E-4</v>
       </c>
     </row>
@@ -15083,11 +15077,11 @@
         <v>3</v>
       </c>
       <c r="E88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9844.5</v>
       </c>
       <c r="F88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.7002805881456651E-4</v>
       </c>
     </row>
@@ -15102,11 +15096,11 @@
         <v>4</v>
       </c>
       <c r="E89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9953</v>
       </c>
       <c r="F89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.6420082219766246E-4</v>
       </c>
     </row>
@@ -15121,11 +15115,11 @@
         <v>5</v>
       </c>
       <c r="E90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10061.5</v>
       </c>
       <c r="F90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5488155675926395E-4</v>
       </c>
     </row>
@@ -15140,11 +15134,11 @@
         <v>6</v>
       </c>
       <c r="E91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10170</v>
       </c>
       <c r="F91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4934024991805974E-4</v>
       </c>
     </row>
@@ -15159,11 +15153,11 @@
         <v>7</v>
       </c>
       <c r="E92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10278.5</v>
       </c>
       <c r="F92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4391593131293474E-4</v>
       </c>
     </row>
@@ -15178,11 +15172,11 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10387</v>
       </c>
       <c r="F93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3685276627836077E-4</v>
       </c>
     </row>
@@ -15197,11 +15191,11 @@
         <v>9</v>
       </c>
       <c r="E94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10495.5</v>
       </c>
       <c r="F94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2993563511346124E-4</v>
       </c>
     </row>
@@ -15216,11 +15210,11 @@
         <v>10</v>
       </c>
       <c r="E95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10604</v>
       </c>
       <c r="F95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2487636898025888E-4</v>
       </c>
     </row>
@@ -15239,7 +15233,7 @@
         <v>10712.5</v>
       </c>
       <c r="F96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1991958693115516E-4</v>
       </c>
     </row>
@@ -15261,7 +15255,7 @@
         <v>10821</v>
       </c>
       <c r="F97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.116984174290731E-4</v>
       </c>
     </row>
@@ -15276,11 +15270,11 @@
         <v>1</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:E108" si="5">($C$109-$C$97)*D98/12+$C$97</f>
+        <f t="shared" ref="E98:E108" si="6">($C$109-$C$97)*D98/12+$C$97</f>
         <v>10931</v>
       </c>
       <c r="F98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0686013478486259E-4</v>
       </c>
     </row>
@@ -15295,11 +15289,11 @@
         <v>2</v>
       </c>
       <c r="E99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11041</v>
       </c>
       <c r="F99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9387635177973002E-4</v>
       </c>
     </row>
@@ -15314,11 +15308,11 @@
         <v>3</v>
       </c>
       <c r="E100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11151</v>
       </c>
       <c r="F100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.8114872731892499E-4</v>
       </c>
     </row>
@@ -15333,11 +15327,11 @@
         <v>4</v>
       </c>
       <c r="E101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11261</v>
       </c>
       <c r="F101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6705357798300929E-4</v>
       </c>
     </row>
@@ -15352,11 +15346,11 @@
         <v>5</v>
       </c>
       <c r="E102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11371</v>
       </c>
       <c r="F102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.516305909770468E-4</v>
       </c>
     </row>
@@ -15371,11 +15365,11 @@
         <v>6</v>
       </c>
       <c r="E103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11481</v>
       </c>
       <c r="F103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3967355703626276E-4</v>
       </c>
     </row>
@@ -15390,11 +15384,11 @@
         <v>7</v>
       </c>
       <c r="E104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11591</v>
       </c>
       <c r="F104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2637330615707592E-4</v>
       </c>
     </row>
@@ -15409,11 +15403,11 @@
         <v>8</v>
       </c>
       <c r="E105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11701</v>
       </c>
       <c r="F105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.117677207076319E-4</v>
       </c>
     </row>
@@ -15428,11 +15422,11 @@
         <v>9</v>
       </c>
       <c r="E106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11811</v>
       </c>
       <c r="F106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.005160242570485E-4</v>
       </c>
     </row>
@@ -15447,11 +15441,11 @@
         <v>10</v>
       </c>
       <c r="E107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11921</v>
       </c>
       <c r="F107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8794527696222358E-4</v>
       </c>
     </row>
@@ -15466,11 +15460,11 @@
         <v>11</v>
       </c>
       <c r="E108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12031</v>
       </c>
       <c r="F108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7409165911672629E-4</v>
       </c>
     </row>
@@ -15492,7 +15486,7 @@
         <v>12141</v>
       </c>
       <c r="F109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6348714390632288E-4</v>
       </c>
     </row>
@@ -15507,11 +15501,11 @@
         <v>1</v>
       </c>
       <c r="E110">
-        <f t="shared" ref="E110:E120" si="6">($C$121-$C$109)*D110/12+$C$109</f>
+        <f t="shared" ref="E110:E120" si="7">($C$121-$C$109)*D110/12+$C$109</f>
         <v>12207.416666666666</v>
       </c>
       <c r="F110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5391380636088724E-4</v>
       </c>
     </row>
@@ -15526,11 +15520,11 @@
         <v>2</v>
       </c>
       <c r="E111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12273.833333333334</v>
       </c>
       <c r="F111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5482375527884523E-4</v>
       </c>
     </row>
@@ -15545,11 +15539,11 @@
         <v>3</v>
       </c>
       <c r="E112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12340.25</v>
       </c>
       <c r="F112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5719873996339894E-4</v>
       </c>
     </row>
@@ -15564,11 +15558,11 @@
         <v>4</v>
       </c>
       <c r="E113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12406.666666666666</v>
       </c>
       <c r="F113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4487894223535743E-4</v>
       </c>
     </row>
@@ -15583,11 +15577,11 @@
         <v>5</v>
       </c>
       <c r="E114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12473.083333333334</v>
       </c>
       <c r="F114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6770932875458492E-4</v>
       </c>
     </row>
@@ -15602,11 +15596,11 @@
         <v>6</v>
       </c>
       <c r="E115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12539.5</v>
       </c>
       <c r="F115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5401297074577677E-4</v>
       </c>
     </row>
@@ -15621,11 +15615,11 @@
         <v>7</v>
       </c>
       <c r="E116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12605.916666666666</v>
       </c>
       <c r="F116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7799840947703124E-4</v>
       </c>
     </row>
@@ -15640,11 +15634,11 @@
         <v>8</v>
       </c>
       <c r="E117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12672.333333333334</v>
       </c>
       <c r="F117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8306206105163479E-4</v>
       </c>
     </row>
@@ -15659,11 +15653,11 @@
         <v>9</v>
       </c>
       <c r="E118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12738.75</v>
       </c>
       <c r="F118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8521552284695646E-4</v>
       </c>
     </row>
@@ -15678,11 +15672,11 @@
         <v>10</v>
       </c>
       <c r="E119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12805.166666666666</v>
       </c>
       <c r="F119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9303178144238659E-4</v>
       </c>
     </row>
@@ -15697,11 +15691,11 @@
         <v>11</v>
       </c>
       <c r="E120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12871.583333333334</v>
       </c>
       <c r="F120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9793947714280157E-4</v>
       </c>
     </row>
@@ -15723,7 +15717,7 @@
         <v>12938</v>
       </c>
       <c r="F121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9998340225176483E-4</v>
       </c>
     </row>
@@ -15738,11 +15732,11 @@
         <v>1</v>
       </c>
       <c r="E122">
-        <f t="shared" ref="E122:E132" si="7">($C$133-$C$121)*D122/12+$C$121</f>
+        <f t="shared" ref="E122:E132" si="8">($C$133-$C$121)*D122/12+$C$121</f>
         <v>13034.166666666666</v>
       </c>
       <c r="F122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0459308611981332E-4</v>
       </c>
     </row>
@@ -15757,11 +15751,11 @@
         <v>2</v>
       </c>
       <c r="E123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13130.333333333334</v>
       </c>
       <c r="F123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.049769871290396E-4</v>
       </c>
     </row>
@@ -15776,11 +15770,11 @@
         <v>3</v>
       </c>
       <c r="E124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13226.5</v>
       </c>
       <c r="F124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0260328822187789E-4</v>
       </c>
     </row>
@@ -15795,11 +15789,11 @@
         <v>4</v>
       </c>
       <c r="E125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13322.666666666666</v>
       </c>
       <c r="F125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.029960099329464E-4</v>
       </c>
     </row>
@@ -15814,11 +15808,11 @@
         <v>5</v>
       </c>
       <c r="E126">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13418.833333333334</v>
       </c>
       <c r="F126">
-        <f t="shared" ref="F126:F189" si="8">B126/E126</f>
+        <f t="shared" ref="F126:F189" si="9">B126/E126</f>
         <v>7.0067052960391489E-4</v>
       </c>
     </row>
@@ -15833,11 +15827,11 @@
         <v>6</v>
       </c>
       <c r="E127">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13515</v>
       </c>
       <c r="F127">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.997247798742138E-4</v>
       </c>
     </row>
@@ -15852,11 +15846,11 @@
         <v>7</v>
       </c>
       <c r="E128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13611.166666666666</v>
       </c>
       <c r="F128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9879239350043477E-4</v>
       </c>
     </row>
@@ -15871,11 +15865,11 @@
         <v>8</v>
       </c>
       <c r="E129">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13707.333333333334</v>
       </c>
       <c r="F129">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9654534981275224E-4</v>
       </c>
     </row>
@@ -15890,11 +15884,11 @@
         <v>9</v>
       </c>
       <c r="E130">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13803.5</v>
       </c>
       <c r="F130">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9696659603240728E-4</v>
       </c>
     </row>
@@ -15909,11 +15903,11 @@
         <v>10</v>
       </c>
       <c r="E131">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13899.666666666666</v>
       </c>
       <c r="F131">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9476327729681771E-4</v>
       </c>
     </row>
@@ -15928,11 +15922,11 @@
         <v>11</v>
       </c>
       <c r="E132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13995.833333333334</v>
       </c>
       <c r="F132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9259023697529028E-4</v>
       </c>
     </row>
@@ -15954,7 +15948,7 @@
         <v>14092</v>
       </c>
       <c r="F133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9302984967830445E-4</v>
       </c>
     </row>
@@ -15969,11 +15963,11 @@
         <v>1</v>
       </c>
       <c r="E134">
-        <f t="shared" ref="E134:E144" si="9">($C$145-$C$133)*D134/12+$C$133</f>
+        <f t="shared" ref="E134:E144" si="10">($C$145-$C$133)*D134/12+$C$133</f>
         <v>14194.25</v>
       </c>
       <c r="F134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9188410682729498E-4</v>
       </c>
       <c r="G134">
@@ -15991,11 +15985,11 @@
         <v>2</v>
       </c>
       <c r="E135">
+        <f t="shared" si="10"/>
+        <v>14296.5</v>
+      </c>
+      <c r="F135">
         <f t="shared" si="9"/>
-        <v>14296.5</v>
-      </c>
-      <c r="F135">
-        <f t="shared" si="8"/>
         <v>6.8820870551067283E-4</v>
       </c>
       <c r="G135">
@@ -16013,11 +16007,11 @@
         <v>3</v>
       </c>
       <c r="E136">
+        <f t="shared" si="10"/>
+        <v>14398.75</v>
+      </c>
+      <c r="F136">
         <f t="shared" si="9"/>
-        <v>14398.75</v>
-      </c>
-      <c r="F136">
-        <f t="shared" si="8"/>
         <v>6.8584948809213755E-4</v>
       </c>
       <c r="G136">
@@ -16035,11 +16029,11 @@
         <v>4</v>
       </c>
       <c r="E137">
+        <f t="shared" si="10"/>
+        <v>14501</v>
+      </c>
+      <c r="F137">
         <f t="shared" si="9"/>
-        <v>14501</v>
-      </c>
-      <c r="F137">
-        <f t="shared" si="8"/>
         <v>6.8101340022527182E-4</v>
       </c>
       <c r="G137" s="2">
@@ -16057,11 +16051,11 @@
         <v>5</v>
       </c>
       <c r="E138">
+        <f t="shared" si="10"/>
+        <v>14603.25</v>
+      </c>
+      <c r="F138">
         <f t="shared" si="9"/>
-        <v>14603.25</v>
-      </c>
-      <c r="F138">
-        <f t="shared" si="8"/>
         <v>6.787376012189068E-4</v>
       </c>
       <c r="G138">
@@ -16079,11 +16073,11 @@
         <v>6</v>
       </c>
       <c r="E139">
+        <f t="shared" si="10"/>
+        <v>14705.5</v>
+      </c>
+      <c r="F139">
         <f t="shared" si="9"/>
-        <v>14705.5</v>
-      </c>
-      <c r="F139">
-        <f t="shared" si="8"/>
         <v>6.7401821597361537E-4</v>
       </c>
       <c r="G139">
@@ -16101,11 +16095,11 @@
         <v>7</v>
       </c>
       <c r="E140">
+        <f t="shared" si="10"/>
+        <v>14807.75</v>
+      </c>
+      <c r="F140">
         <f t="shared" si="9"/>
-        <v>14807.75</v>
-      </c>
-      <c r="F140">
-        <f t="shared" si="8"/>
         <v>6.7182214943751302E-4</v>
       </c>
       <c r="G140">
@@ -16123,11 +16117,11 @@
         <v>8</v>
       </c>
       <c r="E141">
+        <f t="shared" si="10"/>
+        <v>14910</v>
+      </c>
+      <c r="F141">
         <f t="shared" si="9"/>
-        <v>14910</v>
-      </c>
-      <c r="F141">
-        <f t="shared" si="8"/>
         <v>6.6721491839928464E-4</v>
       </c>
       <c r="G141">
@@ -16145,11 +16139,11 @@
         <v>9</v>
       </c>
       <c r="E142">
+        <f t="shared" si="10"/>
+        <v>15012.25</v>
+      </c>
+      <c r="F142">
         <f t="shared" si="9"/>
-        <v>15012.25</v>
-      </c>
-      <c r="F142">
-        <f t="shared" si="8"/>
         <v>6.6509510510860573E-4</v>
       </c>
       <c r="G142">
@@ -16167,11 +16161,11 @@
         <v>10</v>
       </c>
       <c r="E143">
+        <f t="shared" si="10"/>
+        <v>15114.5</v>
+      </c>
+      <c r="F143">
         <f t="shared" si="9"/>
-        <v>15114.5</v>
-      </c>
-      <c r="F143">
-        <f t="shared" si="8"/>
         <v>6.6059571879100636E-4</v>
       </c>
       <c r="G143">
@@ -16189,11 +16183,11 @@
         <v>11</v>
       </c>
       <c r="E144">
+        <f t="shared" si="10"/>
+        <v>15216.75</v>
+      </c>
+      <c r="F144">
         <f t="shared" si="9"/>
-        <v>15216.75</v>
-      </c>
-      <c r="F144">
-        <f t="shared" si="8"/>
         <v>6.5735283596475374E-4</v>
       </c>
       <c r="G144">
@@ -16218,7 +16212,7 @@
         <v>15319</v>
       </c>
       <c r="F145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5415324433709763E-4</v>
       </c>
       <c r="G145">
@@ -16236,11 +16230,11 @@
         <v>1</v>
       </c>
       <c r="E146">
-        <f t="shared" ref="E146:E156" si="10">($C$157-$C$145)*D146/12+$C$145</f>
+        <f t="shared" ref="E146:E156" si="11">($C$157-$C$145)*D146/12+$C$145</f>
         <v>15392.083333333334</v>
       </c>
       <c r="F146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5222966297609703E-4</v>
       </c>
       <c r="G146">
@@ -16258,11 +16252,11 @@
         <v>2</v>
       </c>
       <c r="E147">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15465.166666666666</v>
       </c>
       <c r="F147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5032426259012193E-4</v>
       </c>
       <c r="G147">
@@ -16280,11 +16274,11 @@
         <v>3</v>
       </c>
       <c r="E148">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15538.25</v>
       </c>
       <c r="F148">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4726549697252482E-4</v>
       </c>
       <c r="G148">
@@ -16302,11 +16296,11 @@
         <v>4</v>
       </c>
       <c r="E149">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15611.333333333334</v>
       </c>
       <c r="F149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.465669812529359E-4</v>
       </c>
       <c r="G149">
@@ -16324,11 +16318,11 @@
         <v>5</v>
       </c>
       <c r="E150">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15684.416666666666</v>
       </c>
       <c r="F150">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4355422845393249E-4</v>
       </c>
       <c r="G150">
@@ -16346,11 +16340,11 @@
         <v>6</v>
       </c>
       <c r="E151">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15757.5</v>
       </c>
       <c r="F151">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4287940504521661E-4</v>
       </c>
       <c r="G151">
@@ -16368,11 +16362,11 @@
         <v>7</v>
       </c>
       <c r="E152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15830.583333333334</v>
       </c>
       <c r="F152">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3991149357519998E-4</v>
       </c>
       <c r="G152">
@@ -16390,11 +16384,11 @@
         <v>8</v>
       </c>
       <c r="E153">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15903.666666666666</v>
       </c>
       <c r="F153">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3925961203915242E-4</v>
       </c>
       <c r="G153">
@@ -16412,11 +16406,11 @@
         <v>9</v>
       </c>
       <c r="E154">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15976.75</v>
       </c>
       <c r="F154">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3633541135295563E-4</v>
       </c>
       <c r="G154">
@@ -16434,11 +16428,11 @@
         <v>10</v>
       </c>
       <c r="E155">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16049.833333333334</v>
       </c>
       <c r="F155">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3570575031931793E-4</v>
       </c>
       <c r="G155">
@@ -16456,11 +16450,11 @@
         <v>11</v>
       </c>
       <c r="E156">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16122.916666666666</v>
       </c>
       <c r="F156">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3282416901408456E-4</v>
       </c>
       <c r="G156">
@@ -16485,7 +16479,7 @@
         <v>16196</v>
       </c>
       <c r="F157">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3221603482341315E-4</v>
       </c>
       <c r="G157">
@@ -16503,11 +16497,11 @@
         <v>1</v>
       </c>
       <c r="E158">
-        <f t="shared" ref="E158:E168" si="11">($C$169-$C$157)*D158/12+$C$157</f>
+        <f t="shared" ref="E158:E168" si="12">($C$169-$C$157)*D158/12+$C$157</f>
         <v>16274.25</v>
       </c>
       <c r="F158">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2917620781295603E-4</v>
       </c>
       <c r="G158" s="2">
@@ -16525,11 +16519,11 @@
         <v>2</v>
       </c>
       <c r="E159">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16352.5</v>
       </c>
       <c r="F159">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2839140549355351E-4</v>
       </c>
       <c r="G159">
@@ -16547,11 +16541,11 @@
         <v>3</v>
       </c>
       <c r="E160">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16430.75</v>
       </c>
       <c r="F160">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2761407827802542E-4</v>
       </c>
       <c r="G160">
@@ -16569,11 +16563,11 @@
         <v>4</v>
       </c>
       <c r="E161">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16509</v>
       </c>
       <c r="F161">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2574170402002953E-4</v>
       </c>
       <c r="G161">
@@ -16591,11 +16585,11 @@
         <v>5</v>
       </c>
       <c r="E162">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16587.25</v>
       </c>
       <c r="F162">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2608142599486559E-4</v>
       </c>
       <c r="G162">
@@ -16613,11 +16607,11 @@
         <v>6</v>
       </c>
       <c r="E163">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16665.5</v>
       </c>
       <c r="F163">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2532589431260187E-4</v>
       </c>
       <c r="G163">
@@ -16635,11 +16629,11 @@
         <v>7</v>
       </c>
       <c r="E164">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16743.75</v>
       </c>
       <c r="F164">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2240350528804274E-4</v>
       </c>
       <c r="G164">
@@ -16657,11 +16651,11 @@
         <v>8</v>
       </c>
       <c r="E165">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16822</v>
       </c>
       <c r="F165">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2167211092616808E-4</v>
       </c>
       <c r="G165">
@@ -16679,11 +16673,11 @@
         <v>9</v>
       </c>
       <c r="E166">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16900.25</v>
       </c>
       <c r="F166">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.209474894355606E-4</v>
       </c>
       <c r="G166">
@@ -16701,11 +16695,11 @@
         <v>10</v>
       </c>
       <c r="E167">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16978.5</v>
       </c>
       <c r="F167">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.202295466815875E-4</v>
       </c>
       <c r="G167">
@@ -16723,11 +16717,11 @@
         <v>11</v>
       </c>
       <c r="E168">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>17056.75</v>
       </c>
       <c r="F168">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1951819172272949E-4</v>
       </c>
       <c r="G168">
@@ -16752,7 +16746,7 @@
         <v>17135</v>
       </c>
       <c r="F169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1881333381966729E-4</v>
       </c>
       <c r="G169">
@@ -16770,11 +16764,11 @@
         <v>1</v>
       </c>
       <c r="E170">
-        <f t="shared" ref="E170:E180" si="12">($C$181-$C$169)*D170/12+$C$169</f>
+        <f t="shared" ref="E170:E180" si="13">($C$181-$C$169)*D170/12+$C$169</f>
         <v>17218.833333333332</v>
       </c>
       <c r="F170">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1791445607038806E-4</v>
       </c>
       <c r="G170">
@@ -16792,11 +16786,11 @@
         <v>2</v>
       </c>
       <c r="E171">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17302.666666666668</v>
       </c>
       <c r="F171">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1702428864529547E-4</v>
       </c>
       <c r="G171">
@@ -16814,11 +16808,11 @@
         <v>3</v>
       </c>
       <c r="E172">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17386.5</v>
       </c>
       <c r="F172">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1404915259923888E-4</v>
       </c>
       <c r="G172">
@@ -16836,11 +16830,11 @@
         <v>4</v>
       </c>
       <c r="E173">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17470.333333333332</v>
       </c>
       <c r="F173">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1214432323367226E-4</v>
       </c>
       <c r="G173">
@@ -16858,11 +16852,11 @@
         <v>5</v>
       </c>
       <c r="E174">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17554.166666666668</v>
       </c>
       <c r="F174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1025768715879428E-4</v>
       </c>
       <c r="G174">
@@ -16880,11 +16874,11 @@
         <v>6</v>
       </c>
       <c r="E175">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17638</v>
       </c>
       <c r="F175">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0735713516271695E-4</v>
       </c>
       <c r="G175">
@@ -16902,11 +16896,11 @@
         <v>7</v>
       </c>
       <c r="E176">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17721.833333333332</v>
       </c>
       <c r="F176">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0448402535478844E-4</v>
       </c>
       <c r="G176">
@@ -16924,11 +16918,11 @@
         <v>8</v>
       </c>
       <c r="E177">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17805.666666666668</v>
       </c>
       <c r="F177">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0368223833236602E-4</v>
       </c>
       <c r="G177">
@@ -16946,11 +16940,11 @@
         <v>9</v>
       </c>
       <c r="E178">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17889.5</v>
       </c>
       <c r="F178">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0085327752778628E-4</v>
       </c>
       <c r="G178">
@@ -16968,11 +16962,11 @@
         <v>10</v>
       </c>
       <c r="E179">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17973.333333333332</v>
       </c>
       <c r="F179">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9805070706602371E-4</v>
       </c>
       <c r="G179">
@@ -16990,11 +16984,11 @@
         <v>11</v>
       </c>
       <c r="E180">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>18057.166666666668</v>
       </c>
       <c r="F180">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9628205744718162E-4</v>
       </c>
       <c r="G180">
@@ -17019,7 +17013,7 @@
         <v>18141</v>
       </c>
       <c r="F181">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9452975396431654E-4</v>
       </c>
       <c r="G181">
@@ -17037,11 +17031,11 @@
         <v>1</v>
       </c>
       <c r="E182">
-        <f t="shared" ref="E182:E192" si="13">($C$193-$C$181)*D182/12+$C$181</f>
+        <f t="shared" ref="E182:E192" si="14">($C$193-$C$181)*D182/12+$C$181</f>
         <v>18270.166666666668</v>
       </c>
       <c r="F182">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9032653962288247E-4</v>
       </c>
       <c r="G182">
@@ -17059,11 +17053,11 @@
         <v>2</v>
       </c>
       <c r="E183">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18399.333333333332</v>
       </c>
       <c r="F183">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8618233993985294E-4</v>
       </c>
       <c r="G183">
@@ -17081,11 +17075,11 @@
         <v>3</v>
       </c>
       <c r="E184">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18528.5</v>
       </c>
       <c r="F184">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8406043797393204E-4</v>
       </c>
       <c r="G184">
@@ -17103,11 +17097,11 @@
         <v>4</v>
       </c>
       <c r="E185">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18657.666666666668</v>
       </c>
       <c r="F185">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8196791578082289E-4</v>
       </c>
       <c r="G185">
@@ -17125,11 +17119,11 @@
         <v>5</v>
       </c>
       <c r="E186">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18786.833333333332</v>
       </c>
       <c r="F186">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7990416736899064E-4</v>
       </c>
       <c r="G186">
@@ -17147,11 +17141,11 @@
         <v>6</v>
       </c>
       <c r="E187">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18916</v>
       </c>
       <c r="F187">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7594432975611467E-4</v>
       </c>
       <c r="G187">
@@ -17169,11 +17163,11 @@
         <v>7</v>
       </c>
       <c r="E188">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19045.166666666668</v>
       </c>
       <c r="F188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7394942723875699E-4</v>
       </c>
       <c r="G188">
@@ -17191,11 +17185,11 @@
         <v>8</v>
       </c>
       <c r="E189">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19174.333333333332</v>
       </c>
       <c r="F189">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7198140178711134E-4</v>
       </c>
       <c r="G189">
@@ -17213,11 +17207,11 @@
         <v>9</v>
       </c>
       <c r="E190">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19303.5</v>
       </c>
       <c r="F190">
-        <f t="shared" ref="F190:F205" si="14">B190/E190</f>
+        <f t="shared" ref="F190:F205" si="15">B190/E190</f>
         <v>5.700397138688148E-4</v>
       </c>
       <c r="G190">
@@ -17235,11 +17229,11 @@
         <v>10</v>
       </c>
       <c r="E191">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19432.666666666668</v>
       </c>
       <c r="F191">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.6625072644001504E-4</v>
       </c>
       <c r="G191">
@@ -17257,11 +17251,11 @@
         <v>11</v>
       </c>
       <c r="E192">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19561.833333333332</v>
       </c>
       <c r="F192">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.643725200432816E-4</v>
       </c>
       <c r="G192">
@@ -17286,7 +17280,7 @@
         <v>19691</v>
       </c>
       <c r="F193">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.6251895451390652E-4</v>
       </c>
       <c r="G193">
@@ -17304,11 +17298,11 @@
         <v>1</v>
       </c>
       <c r="E194">
-        <f t="shared" ref="E194:E204" si="15">($C$205-$C$193)*D194/12+$C$193</f>
+        <f t="shared" ref="E194:E204" si="16">($C$205-$C$193)*D194/12+$C$193</f>
         <v>19711.333333333332</v>
       </c>
       <c r="F194">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.6193868502046201E-4</v>
       </c>
       <c r="G194">
@@ -17327,11 +17321,11 @@
         <v>2</v>
       </c>
       <c r="E195">
+        <f t="shared" si="16"/>
+        <v>19731.666666666668</v>
+      </c>
+      <c r="F195">
         <f t="shared" si="15"/>
-        <v>19731.666666666668</v>
-      </c>
-      <c r="F195">
-        <f t="shared" si="14"/>
         <v>5.6320433947123908E-4</v>
       </c>
       <c r="G195">
@@ -17350,11 +17344,11 @@
         <v>3</v>
       </c>
       <c r="E196">
+        <f t="shared" si="16"/>
+        <v>19752</v>
+      </c>
+      <c r="F196">
         <f t="shared" si="15"/>
-        <v>19752</v>
-      </c>
-      <c r="F196">
-        <f t="shared" si="14"/>
         <v>5.6631021710881594E-4</v>
       </c>
       <c r="G196">
@@ -17373,11 +17367,11 @@
         <v>4</v>
       </c>
       <c r="E197">
+        <f t="shared" si="16"/>
+        <v>19772.333333333332</v>
+      </c>
+      <c r="F197">
         <f t="shared" si="15"/>
-        <v>19772.333333333332</v>
-      </c>
-      <c r="F197">
-        <f t="shared" si="14"/>
         <v>5.6756877286444026E-4</v>
       </c>
       <c r="G197">
@@ -17396,11 +17390,11 @@
         <v>5</v>
       </c>
       <c r="E198">
+        <f t="shared" si="16"/>
+        <v>19792.666666666668</v>
+      </c>
+      <c r="F198">
         <f t="shared" si="15"/>
-        <v>19792.666666666668</v>
-      </c>
-      <c r="F198">
-        <f t="shared" si="14"/>
         <v>5.6974426386877282E-4</v>
       </c>
       <c r="G198">
@@ -17419,11 +17413,11 @@
         <v>6</v>
       </c>
       <c r="E199">
+        <f t="shared" si="16"/>
+        <v>19813</v>
+      </c>
+      <c r="F199">
         <f t="shared" si="15"/>
-        <v>19813</v>
-      </c>
-      <c r="F199">
-        <f t="shared" si="14"/>
         <v>5.7191529004525646E-4</v>
       </c>
       <c r="G199">
@@ -17442,11 +17436,11 @@
         <v>7</v>
       </c>
       <c r="E200">
+        <f t="shared" si="16"/>
+        <v>19833.333333333332</v>
+      </c>
+      <c r="F200">
         <f t="shared" si="15"/>
-        <v>19833.333333333332</v>
-      </c>
-      <c r="F200">
-        <f t="shared" si="14"/>
         <v>5.7316422857142863E-4</v>
       </c>
       <c r="G200">
@@ -17465,11 +17459,11 @@
         <v>8</v>
       </c>
       <c r="E201">
+        <f t="shared" si="16"/>
+        <v>19853.666666666668</v>
+      </c>
+      <c r="F201">
         <f t="shared" si="15"/>
-        <v>19853.666666666668</v>
-      </c>
-      <c r="F201">
-        <f t="shared" si="14"/>
         <v>5.7624400110810759E-4</v>
       </c>
       <c r="G201">
@@ -17488,11 +17482,11 @@
         <v>9</v>
       </c>
       <c r="E202">
+        <f t="shared" si="16"/>
+        <v>19874</v>
+      </c>
+      <c r="F202">
         <f t="shared" si="15"/>
-        <v>19874</v>
-      </c>
-      <c r="F202">
-        <f t="shared" si="14"/>
         <v>5.7748595526818962E-4</v>
       </c>
       <c r="G202">
@@ -17511,11 +17505,11 @@
         <v>10</v>
       </c>
       <c r="E203">
+        <f t="shared" si="16"/>
+        <v>19894.333333333332</v>
+      </c>
+      <c r="F203">
         <f t="shared" si="15"/>
-        <v>19894.333333333332</v>
-      </c>
-      <c r="F203">
-        <f t="shared" si="14"/>
         <v>5.7872537070857699E-4</v>
       </c>
       <c r="G203">
@@ -17534,11 +17528,11 @@
         <v>11</v>
       </c>
       <c r="E204">
+        <f t="shared" si="16"/>
+        <v>19914.666666666668</v>
+      </c>
+      <c r="F204">
         <f t="shared" si="15"/>
-        <v>19914.666666666668</v>
-      </c>
-      <c r="F204">
-        <f t="shared" si="14"/>
         <v>5.81790031634976E-4</v>
       </c>
       <c r="G204">
@@ -17562,7 +17556,7 @@
         <v>19935</v>
       </c>
       <c r="F205">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.8302252863472951E-4</v>
       </c>
       <c r="G205">
@@ -23053,7 +23047,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <f>($C$73-$C$61)*D61/12+$C$61</f>
+        <f t="shared" ref="E61:E72" si="1">($C$73-$C$61)*D61/12+$C$61</f>
         <v>7239</v>
       </c>
       <c r="F61">
@@ -23082,11 +23076,11 @@
         <v>1</v>
       </c>
       <c r="E62">
-        <f>($C$73-$C$61)*D62/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7317.25</v>
       </c>
       <c r="F62">
-        <f t="shared" ref="F62:F125" si="1">B62/E62</f>
+        <f t="shared" ref="F62:F125" si="2">B62/E62</f>
         <v>9.5910485621875249E-4</v>
       </c>
       <c r="G62">
@@ -23111,11 +23105,11 @@
         <v>2</v>
       </c>
       <c r="E63">
-        <f>($C$73-$C$61)*D63/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7395.5</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5633957767110632E-4</v>
       </c>
       <c r="G63">
@@ -23140,11 +23134,11 @@
         <v>3</v>
       </c>
       <c r="E64">
-        <f>($C$73-$C$61)*D64/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7473.75</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5606736410771035E-4</v>
       </c>
       <c r="G64">
@@ -23169,11 +23163,11 @@
         <v>4</v>
       </c>
       <c r="E65">
-        <f>($C$73-$C$61)*D65/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7552</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4857100657662428E-4</v>
       </c>
       <c r="G65">
@@ -23198,15 +23192,15 @@
         <v>5</v>
       </c>
       <c r="E66">
-        <f>($C$73-$C$61)*D66/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7630.25</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4599883075041234E-4</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66:G72" si="2">1000*H66</f>
+        <f t="shared" ref="G66:G72" si="3">1000*H66</f>
         <v>0</v>
       </c>
       <c r="I66">
@@ -23227,15 +23221,15 @@
         <v>6</v>
       </c>
       <c r="E67">
-        <f>($C$73-$C$61)*D67/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7708.5</v>
       </c>
       <c r="F67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4347887602430213E-4</v>
       </c>
       <c r="G67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I67">
@@ -23256,15 +23250,15 @@
         <v>7</v>
       </c>
       <c r="E68">
-        <f>($C$73-$C$61)*D68/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7786.75</v>
       </c>
       <c r="F68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3867229256964298E-4</v>
       </c>
       <c r="G68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I68">
@@ -23285,15 +23279,15 @@
         <v>8</v>
       </c>
       <c r="E69">
-        <f>($C$73-$C$61)*D69/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7865</v>
       </c>
       <c r="F69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3627537327823686E-4</v>
       </c>
       <c r="G69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I69">
@@ -23314,15 +23308,15 @@
         <v>9</v>
       </c>
       <c r="E70">
-        <f>($C$73-$C$61)*D70/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>7943.25</v>
       </c>
       <c r="F70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3163445304713646E-4</v>
       </c>
       <c r="G70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I70">
@@ -23343,15 +23337,15 @@
         <v>10</v>
       </c>
       <c r="E71">
-        <f>($C$73-$C$61)*D71/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>8021.5</v>
       </c>
       <c r="F71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2708407737538702E-4</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I71">
@@ -23372,15 +23366,15 @@
         <v>11</v>
       </c>
       <c r="E72">
-        <f>($C$73-$C$61)*D72/12+$C$61</f>
+        <f t="shared" si="1"/>
         <v>8099.75</v>
       </c>
       <c r="F72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2486857793964831E-4</v>
       </c>
       <c r="G72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I72">
@@ -23408,7 +23402,7 @@
         <v>8178</v>
       </c>
       <c r="F73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2492093176815848E-4</v>
       </c>
       <c r="G73">
@@ -23427,11 +23421,11 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <f t="shared" ref="E74:E84" si="3">($C$85-$C$73)*D74/12+$C$73</f>
+        <f t="shared" ref="E74:E84" si="4">($C$85-$C$73)*D74/12+$C$73</f>
         <v>8289.75</v>
       </c>
       <c r="F74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1464798807764616E-4</v>
       </c>
     </row>
@@ -23446,11 +23440,11 @@
         <v>2</v>
       </c>
       <c r="E75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8401.5</v>
       </c>
       <c r="F75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1331334335138564E-4</v>
       </c>
     </row>
@@ -23465,11 +23459,11 @@
         <v>3</v>
       </c>
       <c r="E76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8513.25</v>
       </c>
       <c r="F76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0560028338178711E-4</v>
       </c>
     </row>
@@ -23484,11 +23478,11 @@
         <v>4</v>
       </c>
       <c r="E77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8625</v>
       </c>
       <c r="F77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0019721159420292E-4</v>
       </c>
     </row>
@@ -23503,11 +23497,11 @@
         <v>5</v>
       </c>
       <c r="E78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8736.75</v>
       </c>
       <c r="F78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1368052174244812E-4</v>
       </c>
     </row>
@@ -23522,11 +23516,11 @@
         <v>6</v>
       </c>
       <c r="E79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8848.5</v>
       </c>
       <c r="F79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0831187602418491E-4</v>
       </c>
     </row>
@@ -23541,11 +23535,11 @@
         <v>7</v>
       </c>
       <c r="E80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8960.25</v>
       </c>
       <c r="F80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.051083118030562E-4</v>
       </c>
     </row>
@@ -23560,11 +23554,11 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9072</v>
       </c>
       <c r="F81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0198367146164017E-4</v>
       </c>
     </row>
@@ -23579,11 +23573,11 @@
         <v>9</v>
       </c>
       <c r="E82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9183.75</v>
       </c>
       <c r="F82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9695333650923284E-4</v>
       </c>
     </row>
@@ -23598,11 +23592,11 @@
         <v>10</v>
       </c>
       <c r="E83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9295.5</v>
       </c>
       <c r="F83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9400186335682153E-4</v>
       </c>
     </row>
@@ -23617,11 +23611,11 @@
         <v>11</v>
       </c>
       <c r="E84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9407.25</v>
       </c>
       <c r="F84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9112051166210474E-4</v>
       </c>
     </row>
@@ -23643,7 +23637,7 @@
         <v>9519</v>
       </c>
       <c r="F85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8448292800364194E-4</v>
       </c>
     </row>
@@ -23658,11 +23652,11 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <f t="shared" ref="E86:E95" si="4">($C$97-$C$85)*D86/12+$C$85</f>
+        <f t="shared" ref="E86:E95" si="5">($C$97-$C$85)*D86/12+$C$85</f>
         <v>9627.5</v>
       </c>
       <c r="F86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8207656279754173E-4</v>
       </c>
     </row>
@@ -23677,11 +23671,11 @@
         <v>2</v>
       </c>
       <c r="E87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9736</v>
       </c>
       <c r="F87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.759851752944399E-4</v>
       </c>
     </row>
@@ -23696,11 +23690,11 @@
         <v>3</v>
       </c>
       <c r="E88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9844.5</v>
       </c>
       <c r="F88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.7002805881456651E-4</v>
       </c>
     </row>
@@ -23715,11 +23709,11 @@
         <v>4</v>
       </c>
       <c r="E89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9953</v>
       </c>
       <c r="F89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.6420082219766246E-4</v>
       </c>
     </row>
@@ -23734,11 +23728,11 @@
         <v>5</v>
       </c>
       <c r="E90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10061.5</v>
       </c>
       <c r="F90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5488155675926395E-4</v>
       </c>
     </row>
@@ -23753,11 +23747,11 @@
         <v>6</v>
       </c>
       <c r="E91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10170</v>
       </c>
       <c r="F91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4934024991805974E-4</v>
       </c>
     </row>
@@ -23772,11 +23766,11 @@
         <v>7</v>
       </c>
       <c r="E92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10278.5</v>
       </c>
       <c r="F92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4391593131293474E-4</v>
       </c>
     </row>
@@ -23791,11 +23785,11 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10387</v>
       </c>
       <c r="F93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3685276627836077E-4</v>
       </c>
     </row>
@@ -23810,11 +23804,11 @@
         <v>9</v>
       </c>
       <c r="E94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10495.5</v>
       </c>
       <c r="F94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2993563511346124E-4</v>
       </c>
     </row>
@@ -23829,11 +23823,11 @@
         <v>10</v>
       </c>
       <c r="E95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10604</v>
       </c>
       <c r="F95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2487636898025888E-4</v>
       </c>
     </row>
@@ -23852,7 +23846,7 @@
         <v>10712.5</v>
       </c>
       <c r="F96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1991958693115516E-4</v>
       </c>
     </row>
@@ -23874,7 +23868,7 @@
         <v>10821</v>
       </c>
       <c r="F97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.116984174290731E-4</v>
       </c>
     </row>
@@ -23889,11 +23883,11 @@
         <v>1</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:E108" si="5">($C$109-$C$97)*D98/12+$C$97</f>
+        <f t="shared" ref="E98:E108" si="6">($C$109-$C$97)*D98/12+$C$97</f>
         <v>10931</v>
       </c>
       <c r="F98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0686013478486259E-4</v>
       </c>
     </row>
@@ -23908,11 +23902,11 @@
         <v>2</v>
       </c>
       <c r="E99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11041</v>
       </c>
       <c r="F99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9387635177973002E-4</v>
       </c>
     </row>
@@ -23927,11 +23921,11 @@
         <v>3</v>
       </c>
       <c r="E100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11151</v>
       </c>
       <c r="F100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.8114872731892499E-4</v>
       </c>
     </row>
@@ -23946,11 +23940,11 @@
         <v>4</v>
       </c>
       <c r="E101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11261</v>
       </c>
       <c r="F101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6705357798300929E-4</v>
       </c>
     </row>
@@ -23965,11 +23959,11 @@
         <v>5</v>
       </c>
       <c r="E102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11371</v>
       </c>
       <c r="F102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.516305909770468E-4</v>
       </c>
     </row>
@@ -23984,11 +23978,11 @@
         <v>6</v>
       </c>
       <c r="E103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11481</v>
       </c>
       <c r="F103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3967355703626276E-4</v>
       </c>
     </row>
@@ -24003,11 +23997,11 @@
         <v>7</v>
       </c>
       <c r="E104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11591</v>
       </c>
       <c r="F104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2637330615707592E-4</v>
       </c>
     </row>
@@ -24022,11 +24016,11 @@
         <v>8</v>
       </c>
       <c r="E105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11701</v>
       </c>
       <c r="F105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.117677207076319E-4</v>
       </c>
     </row>
@@ -24041,11 +24035,11 @@
         <v>9</v>
       </c>
       <c r="E106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11811</v>
       </c>
       <c r="F106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.005160242570485E-4</v>
       </c>
     </row>
@@ -24060,11 +24054,11 @@
         <v>10</v>
       </c>
       <c r="E107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11921</v>
       </c>
       <c r="F107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8794527696222358E-4</v>
       </c>
     </row>
@@ -24079,11 +24073,11 @@
         <v>11</v>
       </c>
       <c r="E108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12031</v>
       </c>
       <c r="F108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7409165911672629E-4</v>
       </c>
     </row>
@@ -24105,7 +24099,7 @@
         <v>12141</v>
       </c>
       <c r="F109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6348714390632288E-4</v>
       </c>
     </row>
@@ -24120,11 +24114,11 @@
         <v>1</v>
       </c>
       <c r="E110">
-        <f t="shared" ref="E110:E120" si="6">($C$121-$C$109)*D110/12+$C$109</f>
+        <f t="shared" ref="E110:E120" si="7">($C$121-$C$109)*D110/12+$C$109</f>
         <v>12207.416666666666</v>
       </c>
       <c r="F110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5391380636088724E-4</v>
       </c>
     </row>
@@ -24139,11 +24133,11 @@
         <v>2</v>
       </c>
       <c r="E111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12273.833333333334</v>
       </c>
       <c r="F111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5482375527884523E-4</v>
       </c>
     </row>
@@ -24158,11 +24152,11 @@
         <v>3</v>
       </c>
       <c r="E112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12340.25</v>
       </c>
       <c r="F112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5719873996339894E-4</v>
       </c>
     </row>
@@ -24177,11 +24171,11 @@
         <v>4</v>
       </c>
       <c r="E113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12406.666666666666</v>
       </c>
       <c r="F113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4487894223535743E-4</v>
       </c>
     </row>
@@ -24196,11 +24190,11 @@
         <v>5</v>
       </c>
       <c r="E114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12473.083333333334</v>
       </c>
       <c r="F114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6770932875458492E-4</v>
       </c>
     </row>
@@ -24215,11 +24209,11 @@
         <v>6</v>
       </c>
       <c r="E115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12539.5</v>
       </c>
       <c r="F115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5401297074577677E-4</v>
       </c>
     </row>
@@ -24234,11 +24228,11 @@
         <v>7</v>
       </c>
       <c r="E116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12605.916666666666</v>
       </c>
       <c r="F116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7799840947703124E-4</v>
       </c>
     </row>
@@ -24253,11 +24247,11 @@
         <v>8</v>
       </c>
       <c r="E117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12672.333333333334</v>
       </c>
       <c r="F117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8306206105163479E-4</v>
       </c>
     </row>
@@ -24272,11 +24266,11 @@
         <v>9</v>
       </c>
       <c r="E118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12738.75</v>
       </c>
       <c r="F118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8521552284695646E-4</v>
       </c>
     </row>
@@ -24291,11 +24285,11 @@
         <v>10</v>
       </c>
       <c r="E119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12805.166666666666</v>
       </c>
       <c r="F119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9303178144238659E-4</v>
       </c>
     </row>
@@ -24310,11 +24304,11 @@
         <v>11</v>
       </c>
       <c r="E120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12871.583333333334</v>
       </c>
       <c r="F120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9793947714280157E-4</v>
       </c>
     </row>
@@ -24336,7 +24330,7 @@
         <v>12938</v>
       </c>
       <c r="F121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9998340225176483E-4</v>
       </c>
     </row>
@@ -24351,11 +24345,11 @@
         <v>1</v>
       </c>
       <c r="E122">
-        <f t="shared" ref="E122:E132" si="7">($C$133-$C$121)*D122/12+$C$121</f>
+        <f t="shared" ref="E122:E132" si="8">($C$133-$C$121)*D122/12+$C$121</f>
         <v>13034.166666666666</v>
       </c>
       <c r="F122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0459308611981332E-4</v>
       </c>
     </row>
@@ -24370,11 +24364,11 @@
         <v>2</v>
       </c>
       <c r="E123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13130.333333333334</v>
       </c>
       <c r="F123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.049769871290396E-4</v>
       </c>
     </row>
@@ -24389,11 +24383,11 @@
         <v>3</v>
       </c>
       <c r="E124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13226.5</v>
       </c>
       <c r="F124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0260328822187789E-4</v>
       </c>
     </row>
@@ -24408,11 +24402,11 @@
         <v>4</v>
       </c>
       <c r="E125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13322.666666666666</v>
       </c>
       <c r="F125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.029960099329464E-4</v>
       </c>
     </row>
@@ -24427,11 +24421,11 @@
         <v>5</v>
       </c>
       <c r="E126">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13418.833333333334</v>
       </c>
       <c r="F126">
-        <f t="shared" ref="F126:F189" si="8">B126/E126</f>
+        <f t="shared" ref="F126:F189" si="9">B126/E126</f>
         <v>7.0067052960391489E-4</v>
       </c>
     </row>
@@ -24446,11 +24440,11 @@
         <v>6</v>
       </c>
       <c r="E127">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13515</v>
       </c>
       <c r="F127">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.997247798742138E-4</v>
       </c>
     </row>
@@ -24465,11 +24459,11 @@
         <v>7</v>
       </c>
       <c r="E128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13611.166666666666</v>
       </c>
       <c r="F128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9879239350043477E-4</v>
       </c>
     </row>
@@ -24484,11 +24478,11 @@
         <v>8</v>
       </c>
       <c r="E129">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13707.333333333334</v>
       </c>
       <c r="F129">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9654534981275224E-4</v>
       </c>
     </row>
@@ -24503,11 +24497,11 @@
         <v>9</v>
       </c>
       <c r="E130">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13803.5</v>
       </c>
       <c r="F130">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9696659603240728E-4</v>
       </c>
     </row>
@@ -24522,11 +24516,11 @@
         <v>10</v>
       </c>
       <c r="E131">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13899.666666666666</v>
       </c>
       <c r="F131">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9476327729681771E-4</v>
       </c>
     </row>
@@ -24541,11 +24535,11 @@
         <v>11</v>
       </c>
       <c r="E132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13995.833333333334</v>
       </c>
       <c r="F132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9259023697529028E-4</v>
       </c>
     </row>
@@ -24567,7 +24561,7 @@
         <v>14092</v>
       </c>
       <c r="F133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9302984967830445E-4</v>
       </c>
     </row>
@@ -24582,11 +24576,11 @@
         <v>1</v>
       </c>
       <c r="E134">
-        <f t="shared" ref="E134:E144" si="9">($C$145-$C$133)*D134/12+$C$133</f>
+        <f t="shared" ref="E134:E144" si="10">($C$145-$C$133)*D134/12+$C$133</f>
         <v>14194.25</v>
       </c>
       <c r="F134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.9188410682729498E-4</v>
       </c>
       <c r="G134" s="8">
@@ -24604,11 +24598,11 @@
         <v>2</v>
       </c>
       <c r="E135">
+        <f t="shared" si="10"/>
+        <v>14296.5</v>
+      </c>
+      <c r="F135">
         <f t="shared" si="9"/>
-        <v>14296.5</v>
-      </c>
-      <c r="F135">
-        <f t="shared" si="8"/>
         <v>6.8820870551067283E-4</v>
       </c>
       <c r="G135" s="8">
@@ -24626,11 +24620,11 @@
         <v>3</v>
       </c>
       <c r="E136">
+        <f t="shared" si="10"/>
+        <v>14398.75</v>
+      </c>
+      <c r="F136">
         <f t="shared" si="9"/>
-        <v>14398.75</v>
-      </c>
-      <c r="F136">
-        <f t="shared" si="8"/>
         <v>6.8584948809213755E-4</v>
       </c>
       <c r="G136" s="8">
@@ -24648,11 +24642,11 @@
         <v>4</v>
       </c>
       <c r="E137">
+        <f t="shared" si="10"/>
+        <v>14501</v>
+      </c>
+      <c r="F137">
         <f t="shared" si="9"/>
-        <v>14501</v>
-      </c>
-      <c r="F137">
-        <f t="shared" si="8"/>
         <v>6.8101340022527182E-4</v>
       </c>
       <c r="G137" s="8">
@@ -24670,11 +24664,11 @@
         <v>5</v>
       </c>
       <c r="E138">
+        <f t="shared" si="10"/>
+        <v>14603.25</v>
+      </c>
+      <c r="F138">
         <f t="shared" si="9"/>
-        <v>14603.25</v>
-      </c>
-      <c r="F138">
-        <f t="shared" si="8"/>
         <v>6.787376012189068E-4</v>
       </c>
       <c r="G138" s="8">
@@ -24692,11 +24686,11 @@
         <v>6</v>
       </c>
       <c r="E139">
+        <f t="shared" si="10"/>
+        <v>14705.5</v>
+      </c>
+      <c r="F139">
         <f t="shared" si="9"/>
-        <v>14705.5</v>
-      </c>
-      <c r="F139">
-        <f t="shared" si="8"/>
         <v>6.7401821597361537E-4</v>
       </c>
       <c r="G139" s="8">
@@ -24714,11 +24708,11 @@
         <v>7</v>
       </c>
       <c r="E140">
+        <f t="shared" si="10"/>
+        <v>14807.75</v>
+      </c>
+      <c r="F140">
         <f t="shared" si="9"/>
-        <v>14807.75</v>
-      </c>
-      <c r="F140">
-        <f t="shared" si="8"/>
         <v>6.7182214943751302E-4</v>
       </c>
       <c r="G140" s="8">
@@ -24736,11 +24730,11 @@
         <v>8</v>
       </c>
       <c r="E141">
+        <f t="shared" si="10"/>
+        <v>14910</v>
+      </c>
+      <c r="F141">
         <f t="shared" si="9"/>
-        <v>14910</v>
-      </c>
-      <c r="F141">
-        <f t="shared" si="8"/>
         <v>6.6721491839928464E-4</v>
       </c>
       <c r="G141" s="8">
@@ -24758,11 +24752,11 @@
         <v>9</v>
       </c>
       <c r="E142">
+        <f t="shared" si="10"/>
+        <v>15012.25</v>
+      </c>
+      <c r="F142">
         <f t="shared" si="9"/>
-        <v>15012.25</v>
-      </c>
-      <c r="F142">
-        <f t="shared" si="8"/>
         <v>6.6509510510860573E-4</v>
       </c>
       <c r="G142" s="8">
@@ -24780,11 +24774,11 @@
         <v>10</v>
       </c>
       <c r="E143">
+        <f t="shared" si="10"/>
+        <v>15114.5</v>
+      </c>
+      <c r="F143">
         <f t="shared" si="9"/>
-        <v>15114.5</v>
-      </c>
-      <c r="F143">
-        <f t="shared" si="8"/>
         <v>6.6059571879100636E-4</v>
       </c>
       <c r="G143" s="8">
@@ -24802,11 +24796,11 @@
         <v>11</v>
       </c>
       <c r="E144">
+        <f t="shared" si="10"/>
+        <v>15216.75</v>
+      </c>
+      <c r="F144">
         <f t="shared" si="9"/>
-        <v>15216.75</v>
-      </c>
-      <c r="F144">
-        <f t="shared" si="8"/>
         <v>6.5735283596475374E-4</v>
       </c>
       <c r="G144" s="8">
@@ -24831,7 +24825,7 @@
         <v>15319</v>
       </c>
       <c r="F145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5415324433709763E-4</v>
       </c>
       <c r="G145" s="8">
@@ -24849,11 +24843,11 @@
         <v>1</v>
       </c>
       <c r="E146">
-        <f t="shared" ref="E146:E156" si="10">($C$157-$C$145)*D146/12+$C$145</f>
+        <f t="shared" ref="E146:E156" si="11">($C$157-$C$145)*D146/12+$C$145</f>
         <v>15392.083333333334</v>
       </c>
       <c r="F146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5222966297609703E-4</v>
       </c>
       <c r="G146" s="8">
@@ -24871,11 +24865,11 @@
         <v>2</v>
       </c>
       <c r="E147">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15465.166666666666</v>
       </c>
       <c r="F147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.5032426259012193E-4</v>
       </c>
       <c r="G147" s="8">
@@ -24893,11 +24887,11 @@
         <v>3</v>
       </c>
       <c r="E148">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15538.25</v>
       </c>
       <c r="F148">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4726549697252482E-4</v>
       </c>
       <c r="G148" s="8">
@@ -24915,11 +24909,11 @@
         <v>4</v>
       </c>
       <c r="E149">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15611.333333333334</v>
       </c>
       <c r="F149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.465669812529359E-4</v>
       </c>
       <c r="G149" s="8">
@@ -24937,11 +24931,11 @@
         <v>5</v>
       </c>
       <c r="E150">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15684.416666666666</v>
       </c>
       <c r="F150">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4355422845393249E-4</v>
       </c>
       <c r="G150" s="8">
@@ -24959,11 +24953,11 @@
         <v>6</v>
       </c>
       <c r="E151">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15757.5</v>
       </c>
       <c r="F151">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4287940504521661E-4</v>
       </c>
       <c r="G151" s="8">
@@ -24981,11 +24975,11 @@
         <v>7</v>
       </c>
       <c r="E152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15830.583333333334</v>
       </c>
       <c r="F152">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3991149357519998E-4</v>
       </c>
       <c r="G152" s="8">
@@ -25003,11 +24997,11 @@
         <v>8</v>
       </c>
       <c r="E153">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15903.666666666666</v>
       </c>
       <c r="F153">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3925961203915242E-4</v>
       </c>
       <c r="G153" s="8">
@@ -25025,11 +25019,11 @@
         <v>9</v>
       </c>
       <c r="E154">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15976.75</v>
       </c>
       <c r="F154">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3633541135295563E-4</v>
       </c>
       <c r="G154" s="8">
@@ -25047,11 +25041,11 @@
         <v>10</v>
       </c>
       <c r="E155">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16049.833333333334</v>
       </c>
       <c r="F155">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3570575031931793E-4</v>
       </c>
       <c r="G155" s="8">
@@ -25069,11 +25063,11 @@
         <v>11</v>
       </c>
       <c r="E156">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16122.916666666666</v>
       </c>
       <c r="F156">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3282416901408456E-4</v>
       </c>
       <c r="G156" s="8">
@@ -25098,7 +25092,7 @@
         <v>16196</v>
       </c>
       <c r="F157">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3221603482341315E-4</v>
       </c>
       <c r="G157" s="8">
@@ -25116,11 +25110,11 @@
         <v>1</v>
       </c>
       <c r="E158">
-        <f t="shared" ref="E158:E168" si="11">($C$169-$C$157)*D158/12+$C$157</f>
+        <f t="shared" ref="E158:E168" si="12">($C$169-$C$157)*D158/12+$C$157</f>
         <v>16274.25</v>
       </c>
       <c r="F158">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2917620781295603E-4</v>
       </c>
       <c r="G158" s="8">
@@ -25138,11 +25132,11 @@
         <v>2</v>
       </c>
       <c r="E159">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16352.5</v>
       </c>
       <c r="F159">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2839140549355351E-4</v>
       </c>
       <c r="G159" s="8">
@@ -25160,11 +25154,11 @@
         <v>3</v>
       </c>
       <c r="E160">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16430.75</v>
       </c>
       <c r="F160">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2761407827802542E-4</v>
       </c>
       <c r="G160" s="8">
@@ -25182,11 +25176,11 @@
         <v>4</v>
       </c>
       <c r="E161">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16509</v>
       </c>
       <c r="F161">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2574170402002953E-4</v>
       </c>
       <c r="G161" s="8">
@@ -25204,11 +25198,11 @@
         <v>5</v>
       </c>
       <c r="E162">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16587.25</v>
       </c>
       <c r="F162">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2608142599486559E-4</v>
       </c>
       <c r="G162" s="8">
@@ -25226,11 +25220,11 @@
         <v>6</v>
       </c>
       <c r="E163">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16665.5</v>
       </c>
       <c r="F163">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2532589431260187E-4</v>
       </c>
       <c r="G163" s="8">
@@ -25248,11 +25242,11 @@
         <v>7</v>
       </c>
       <c r="E164">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16743.75</v>
       </c>
       <c r="F164">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2240350528804274E-4</v>
       </c>
       <c r="G164" s="8">
@@ -25270,11 +25264,11 @@
         <v>8</v>
       </c>
       <c r="E165">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16822</v>
       </c>
       <c r="F165">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2167211092616808E-4</v>
       </c>
       <c r="G165" s="8">
@@ -25292,11 +25286,11 @@
         <v>9</v>
       </c>
       <c r="E166">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16900.25</v>
       </c>
       <c r="F166">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.209474894355606E-4</v>
       </c>
       <c r="G166" s="8">
@@ -25314,11 +25308,11 @@
         <v>10</v>
       </c>
       <c r="E167">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>16978.5</v>
       </c>
       <c r="F167">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.202295466815875E-4</v>
       </c>
       <c r="G167" s="8">
@@ -25336,11 +25330,11 @@
         <v>11</v>
       </c>
       <c r="E168">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>17056.75</v>
       </c>
       <c r="F168">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1951819172272949E-4</v>
       </c>
       <c r="G168" s="8">
@@ -25365,7 +25359,7 @@
         <v>17135</v>
       </c>
       <c r="F169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1881333381966729E-4</v>
       </c>
       <c r="G169" s="8">
@@ -25383,11 +25377,11 @@
         <v>1</v>
       </c>
       <c r="E170">
-        <f t="shared" ref="E170:E180" si="12">($C$181-$C$169)*D170/12+$C$169</f>
+        <f t="shared" ref="E170:E180" si="13">($C$181-$C$169)*D170/12+$C$169</f>
         <v>17218.833333333332</v>
       </c>
       <c r="F170">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1791445607038806E-4</v>
       </c>
       <c r="G170" s="8">
@@ -25405,11 +25399,11 @@
         <v>2</v>
       </c>
       <c r="E171">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17302.666666666668</v>
       </c>
       <c r="F171">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1702428864529547E-4</v>
       </c>
       <c r="G171" s="8">
@@ -25427,11 +25421,11 @@
         <v>3</v>
       </c>
       <c r="E172">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17386.5</v>
       </c>
       <c r="F172">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1404915259923888E-4</v>
       </c>
       <c r="G172" s="8">
@@ -25449,11 +25443,11 @@
         <v>4</v>
       </c>
       <c r="E173">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17470.333333333332</v>
       </c>
       <c r="F173">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1214432323367226E-4</v>
       </c>
       <c r="G173" s="8">
@@ -25471,11 +25465,11 @@
         <v>5</v>
       </c>
       <c r="E174">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17554.166666666668</v>
       </c>
       <c r="F174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.1025768715879428E-4</v>
       </c>
       <c r="G174" s="8">
@@ -25493,11 +25487,11 @@
         <v>6</v>
       </c>
       <c r="E175">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17638</v>
       </c>
       <c r="F175">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0735713516271695E-4</v>
       </c>
       <c r="G175" s="8">
@@ -25515,11 +25509,11 @@
         <v>7</v>
       </c>
       <c r="E176">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17721.833333333332</v>
       </c>
       <c r="F176">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0448402535478844E-4</v>
       </c>
       <c r="G176" s="8">
@@ -25537,11 +25531,11 @@
         <v>8</v>
       </c>
       <c r="E177">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17805.666666666668</v>
       </c>
       <c r="F177">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0368223833236602E-4</v>
       </c>
       <c r="G177" s="8">
@@ -25559,11 +25553,11 @@
         <v>9</v>
       </c>
       <c r="E178">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17889.5</v>
       </c>
       <c r="F178">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0085327752778628E-4</v>
       </c>
       <c r="G178" s="8">
@@ -25581,11 +25575,11 @@
         <v>10</v>
       </c>
       <c r="E179">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17973.333333333332</v>
       </c>
       <c r="F179">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9805070706602371E-4</v>
       </c>
       <c r="G179" s="8">
@@ -25603,11 +25597,11 @@
         <v>11</v>
       </c>
       <c r="E180">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>18057.166666666668</v>
       </c>
       <c r="F180">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9628205744718162E-4</v>
       </c>
       <c r="G180" s="8">
@@ -25632,7 +25626,7 @@
         <v>18141</v>
       </c>
       <c r="F181">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9452975396431654E-4</v>
       </c>
       <c r="G181" s="8">
@@ -25650,11 +25644,11 @@
         <v>1</v>
       </c>
       <c r="E182">
-        <f t="shared" ref="E182:E192" si="13">($C$193-$C$181)*D182/12+$C$181</f>
+        <f t="shared" ref="E182:E192" si="14">($C$193-$C$181)*D182/12+$C$181</f>
         <v>18270.166666666668</v>
       </c>
       <c r="F182">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.9032653962288247E-4</v>
       </c>
       <c r="G182" s="8">
@@ -25672,11 +25666,11 @@
         <v>2</v>
       </c>
       <c r="E183">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18399.333333333332</v>
       </c>
       <c r="F183">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8618233993985294E-4</v>
       </c>
       <c r="G183" s="8">
@@ -25694,11 +25688,11 @@
         <v>3</v>
       </c>
       <c r="E184">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18528.5</v>
       </c>
       <c r="F184">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8406043797393204E-4</v>
       </c>
       <c r="G184" s="8">
@@ -25716,11 +25710,11 @@
         <v>4</v>
       </c>
       <c r="E185">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18657.666666666668</v>
       </c>
       <c r="F185">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8196791578082289E-4</v>
       </c>
       <c r="G185" s="8">
@@ -25738,11 +25732,11 @@
         <v>5</v>
       </c>
       <c r="E186">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18786.833333333332</v>
       </c>
       <c r="F186">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7990416736899064E-4</v>
       </c>
       <c r="G186" s="8">
@@ -25760,11 +25754,11 @@
         <v>6</v>
       </c>
       <c r="E187">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18916</v>
       </c>
       <c r="F187">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7594432975611467E-4</v>
       </c>
       <c r="G187" s="8">
@@ -25782,11 +25776,11 @@
         <v>7</v>
       </c>
       <c r="E188">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19045.166666666668</v>
       </c>
       <c r="F188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7394942723875699E-4</v>
       </c>
       <c r="G188" s="8">
@@ -25804,11 +25798,11 @@
         <v>8</v>
       </c>
       <c r="E189">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19174.333333333332</v>
       </c>
       <c r="F189">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.7198140178711134E-4</v>
       </c>
       <c r="G189" s="8">
@@ -25826,11 +25820,11 @@
         <v>9</v>
       </c>
       <c r="E190">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19303.5</v>
       </c>
       <c r="F190">
-        <f t="shared" ref="F190:F205" si="14">B190/E190</f>
+        <f t="shared" ref="F190:F205" si="15">B190/E190</f>
         <v>5.700397138688148E-4</v>
       </c>
       <c r="G190" s="8">
@@ -25848,11 +25842,11 @@
         <v>10</v>
       </c>
       <c r="E191">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19432.666666666668</v>
       </c>
       <c r="F191">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.6625072644001504E-4</v>
       </c>
       <c r="G191" s="8">
@@ -25870,11 +25864,11 @@
         <v>11</v>
       </c>
       <c r="E192">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19561.833333333332</v>
       </c>
       <c r="F192">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.643725200432816E-4</v>
       </c>
       <c r="G192" s="8">
@@ -25899,7 +25893,7 @@
         <v>19691</v>
       </c>
       <c r="F193">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.6251895451390652E-4</v>
       </c>
       <c r="G193" s="8">
@@ -25917,11 +25911,11 @@
         <v>1</v>
       </c>
       <c r="E194">
-        <f t="shared" ref="E194:E204" si="15">($C$205-$C$193)*D194/12+$C$193</f>
+        <f t="shared" ref="E194:E204" si="16">($C$205-$C$193)*D194/12+$C$193</f>
         <v>19711.333333333332</v>
       </c>
       <c r="F194">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.6193868502046201E-4</v>
       </c>
       <c r="G194" s="8">
@@ -25940,11 +25934,11 @@
         <v>2</v>
       </c>
       <c r="E195">
+        <f t="shared" si="16"/>
+        <v>19731.666666666668</v>
+      </c>
+      <c r="F195">
         <f t="shared" si="15"/>
-        <v>19731.666666666668</v>
-      </c>
-      <c r="F195">
-        <f t="shared" si="14"/>
         <v>5.6320433947123908E-4</v>
       </c>
       <c r="G195" s="8">
@@ -25963,11 +25957,11 @@
         <v>3</v>
       </c>
       <c r="E196">
+        <f t="shared" si="16"/>
+        <v>19752</v>
+      </c>
+      <c r="F196">
         <f t="shared" si="15"/>
-        <v>19752</v>
-      </c>
-      <c r="F196">
-        <f t="shared" si="14"/>
         <v>5.6631021710881594E-4</v>
       </c>
       <c r="G196" s="8">
@@ -25986,11 +25980,11 @@
         <v>4</v>
       </c>
       <c r="E197">
+        <f t="shared" si="16"/>
+        <v>19772.333333333332</v>
+      </c>
+      <c r="F197">
         <f t="shared" si="15"/>
-        <v>19772.333333333332</v>
-      </c>
-      <c r="F197">
-        <f t="shared" si="14"/>
         <v>5.6756877286444026E-4</v>
       </c>
       <c r="G197" s="8">
@@ -26009,11 +26003,11 @@
         <v>5</v>
       </c>
       <c r="E198">
+        <f t="shared" si="16"/>
+        <v>19792.666666666668</v>
+      </c>
+      <c r="F198">
         <f t="shared" si="15"/>
-        <v>19792.666666666668</v>
-      </c>
-      <c r="F198">
-        <f t="shared" si="14"/>
         <v>5.6974426386877282E-4</v>
       </c>
       <c r="G198" s="8">
@@ -26032,11 +26026,11 @@
         <v>6</v>
       </c>
       <c r="E199">
+        <f t="shared" si="16"/>
+        <v>19813</v>
+      </c>
+      <c r="F199">
         <f t="shared" si="15"/>
-        <v>19813</v>
-      </c>
-      <c r="F199">
-        <f t="shared" si="14"/>
         <v>5.7191529004525646E-4</v>
       </c>
       <c r="G199" s="8">
@@ -26055,11 +26049,11 @@
         <v>7</v>
       </c>
       <c r="E200">
+        <f t="shared" si="16"/>
+        <v>19833.333333333332</v>
+      </c>
+      <c r="F200">
         <f t="shared" si="15"/>
-        <v>19833.333333333332</v>
-      </c>
-      <c r="F200">
-        <f t="shared" si="14"/>
         <v>5.7316422857142863E-4</v>
       </c>
       <c r="G200" s="8">
@@ -26078,11 +26072,11 @@
         <v>8</v>
       </c>
       <c r="E201">
+        <f t="shared" si="16"/>
+        <v>19853.666666666668</v>
+      </c>
+      <c r="F201">
         <f t="shared" si="15"/>
-        <v>19853.666666666668</v>
-      </c>
-      <c r="F201">
-        <f t="shared" si="14"/>
         <v>5.7624400110810759E-4</v>
       </c>
       <c r="G201" s="8">
@@ -26101,11 +26095,11 @@
         <v>9</v>
       </c>
       <c r="E202">
+        <f t="shared" si="16"/>
+        <v>19874</v>
+      </c>
+      <c r="F202">
         <f t="shared" si="15"/>
-        <v>19874</v>
-      </c>
-      <c r="F202">
-        <f t="shared" si="14"/>
         <v>5.7748595526818962E-4</v>
       </c>
       <c r="G202" s="8">
@@ -26124,11 +26118,11 @@
         <v>10</v>
       </c>
       <c r="E203">
+        <f t="shared" si="16"/>
+        <v>19894.333333333332</v>
+      </c>
+      <c r="F203">
         <f t="shared" si="15"/>
-        <v>19894.333333333332</v>
-      </c>
-      <c r="F203">
-        <f t="shared" si="14"/>
         <v>5.7872537070857699E-4</v>
       </c>
       <c r="G203" s="8">
@@ -26147,11 +26141,11 @@
         <v>11</v>
       </c>
       <c r="E204">
+        <f t="shared" si="16"/>
+        <v>19914.666666666668</v>
+      </c>
+      <c r="F204">
         <f t="shared" si="15"/>
-        <v>19914.666666666668</v>
-      </c>
-      <c r="F204">
-        <f t="shared" si="14"/>
         <v>5.81790031634976E-4</v>
       </c>
       <c r="G204" s="8">
@@ -26175,7 +26169,7 @@
         <v>19935</v>
       </c>
       <c r="F205">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.8302252863472951E-4</v>
       </c>
       <c r="G205" s="8">

</xml_diff>

<commit_message>
add two market scenario
</commit_message>
<xml_diff>
--- a/data/correlation/ship_demand_month.xlsx
+++ b/data/correlation/ship_demand_month.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9025E32-2B38-8C41-A5CF-217172A097C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8A4DA9-9BF9-314C-A9B1-5F4E34E8B731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
   </bookViews>
   <sheets>
     <sheet name="海事センター" sheetId="5" r:id="rId1"/>
     <sheet name="行き（月）" sheetId="8" r:id="rId2"/>
     <sheet name="行き（コンテナ積載数）" sheetId="10" r:id="rId3"/>
-    <sheet name="帰り（月）" sheetId="9" r:id="rId4"/>
-    <sheet name="帰り（コンテナ積載数）" sheetId="11" r:id="rId5"/>
-    <sheet name="行き" sheetId="6" r:id="rId6"/>
-    <sheet name="帰り" sheetId="7" r:id="rId7"/>
+    <sheet name="行き（原油追加）" sheetId="12" r:id="rId4"/>
+    <sheet name="帰り（月）" sheetId="9" r:id="rId5"/>
+    <sheet name="帰り（コンテナ積載数）" sheetId="11" r:id="rId6"/>
+    <sheet name="行き" sheetId="6" r:id="rId7"/>
+    <sheet name="帰り" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
   <si>
     <t>Gap</t>
     <phoneticPr fontId="1"/>
@@ -542,6 +543,16 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>X 値 2</t>
+  </si>
+  <si>
+    <t>原油あり</t>
+    <rPh sb="0" eb="1">
+      <t>ゲンユア</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -626,7 +637,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -654,6 +665,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -8592,7 +8604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35A8DBA-102A-6246-87AB-BC7138704158}">
   <dimension ref="A1:Y216"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection sqref="A1:E204"/>
     </sheetView>
   </sheetViews>
@@ -13027,8 +13039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40FD581-74FB-F94A-9780-764D633DA0D6}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="107" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134:G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -17626,6 +17638,2441 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7311AD3-701D-CE48-8EB0-A330C275BCB3}">
+  <dimension ref="A1:N234"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="H154" sqref="H154"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1">
+        <v>36557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1">
+        <v>36586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1">
+        <v>36647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1">
+        <v>36678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1">
+        <v>36708</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1">
+        <v>36739</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1">
+        <v>36770</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1">
+        <v>36800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1">
+        <v>36831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1">
+        <v>36861</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1">
+        <v>36923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1">
+        <v>36951</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1">
+        <v>36982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1">
+        <v>37012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1">
+        <v>37043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1">
+        <v>37073</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1">
+        <v>37104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1">
+        <v>37135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1">
+        <v>37165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1">
+        <v>37196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1">
+        <v>37226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1">
+        <v>37288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1">
+        <v>37316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1">
+        <v>37347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1">
+        <v>37377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1">
+        <v>37408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1">
+        <v>37438</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1">
+        <v>37469</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1">
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1">
+        <v>37530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1">
+        <v>37561</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1">
+        <v>37591</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1">
+        <v>37622</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1">
+        <v>37653</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="1">
+        <v>37681</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="1">
+        <v>37712</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1">
+        <v>37742</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1">
+        <v>37773</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1">
+        <v>37803</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1">
+        <v>37834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="1">
+        <v>37865</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1">
+        <v>37895</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="1">
+        <v>37926</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1">
+        <v>37956</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1">
+        <v>38018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="1">
+        <v>38047</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="1">
+        <v>38078</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="1">
+        <v>38108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="1">
+        <v>38139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="1">
+        <v>38169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="1">
+        <v>38200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="1">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="1">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="1">
+        <v>38292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="1">
+        <v>38322</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="1">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="1">
+        <v>38384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="1">
+        <v>38412</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1">
+        <v>38443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="1">
+        <v>38473</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="1">
+        <v>38504</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="1">
+        <v>38534</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="1">
+        <v>38565</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="1">
+        <v>38596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="1">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="1">
+        <v>38657</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="1">
+        <v>38687</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="1">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="1">
+        <v>38749</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="1">
+        <v>38777</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="1">
+        <v>38808</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="1">
+        <v>38838</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="1">
+        <v>38869</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="1">
+        <v>38899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="1">
+        <v>38930</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="1">
+        <v>38961</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="1">
+        <v>38991</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="1">
+        <v>39022</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="1">
+        <v>39052</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="1">
+        <v>39083</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="1">
+        <v>39114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1">
+        <v>39142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="1">
+        <v>39173</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="1">
+        <v>39203</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="1">
+        <v>39234</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="1">
+        <v>39264</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="1">
+        <v>39295</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="1">
+        <v>39326</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="1">
+        <v>39356</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="1">
+        <v>39387</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="1">
+        <v>39417</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1">
+        <v>39479</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="1">
+        <v>39508</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="1">
+        <v>39539</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="1">
+        <v>39569</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="1">
+        <v>39600</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="1">
+        <v>39630</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="1">
+        <v>39661</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1">
+        <v>39692</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1">
+        <v>39722</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="1">
+        <v>39753</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="1">
+        <v>39783</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1">
+        <v>39814</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="1">
+        <v>39845</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1">
+        <v>39873</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1">
+        <v>39904</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1">
+        <v>39934</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1">
+        <v>39965</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1">
+        <v>39995</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="1">
+        <v>40026</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1">
+        <v>40057</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="1">
+        <v>40087</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="1">
+        <v>40118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1">
+        <v>40148</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="1">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1">
+        <v>40210</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="1">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="1">
+        <v>40269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1">
+        <v>40299</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="1">
+        <v>40330</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="1">
+        <v>40360</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="1">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="1">
+        <v>40422</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="1">
+        <v>40452</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1">
+        <v>40483</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="1">
+        <v>40513</v>
+      </c>
+      <c r="F133" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="1">
+        <v>40544</v>
+      </c>
+      <c r="B134">
+        <v>6.9188410682729498E-4</v>
+      </c>
+      <c r="C134">
+        <v>1660</v>
+      </c>
+      <c r="D134">
+        <v>89.17</v>
+      </c>
+      <c r="E134">
+        <v>6.9188410682729498E-4</v>
+      </c>
+      <c r="F134" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="21" thickBot="1">
+      <c r="A135" s="1">
+        <v>40575</v>
+      </c>
+      <c r="B135">
+        <v>6.8820870551067283E-4</v>
+      </c>
+      <c r="C135">
+        <v>1760</v>
+      </c>
+      <c r="D135">
+        <v>88.58</v>
+      </c>
+      <c r="E135">
+        <v>6.8820870551067283E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="A136" s="1">
+        <v>40603</v>
+      </c>
+      <c r="B136">
+        <v>6.8584948809213755E-4</v>
+      </c>
+      <c r="C136">
+        <v>1840</v>
+      </c>
+      <c r="D136">
+        <v>102.86</v>
+      </c>
+      <c r="E136">
+        <v>6.8584948809213755E-4</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" s="6"/>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="A137" s="1">
+        <v>40634</v>
+      </c>
+      <c r="B137">
+        <v>6.8101340022527182E-4</v>
+      </c>
+      <c r="C137">
+        <v>1880</v>
+      </c>
+      <c r="D137">
+        <v>109.53</v>
+      </c>
+      <c r="E137">
+        <v>6.8101340022527182E-4</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G137" s="3">
+        <v>0.70723892278498079</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="A138" s="1">
+        <v>40664</v>
+      </c>
+      <c r="B138">
+        <v>6.787376012189068E-4</v>
+      </c>
+      <c r="C138">
+        <v>1790</v>
+      </c>
+      <c r="D138">
+        <v>100.9</v>
+      </c>
+      <c r="E138">
+        <v>6.787376012189068E-4</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G138" s="3">
+        <v>0.50018689390206006</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" s="1">
+        <v>40695</v>
+      </c>
+      <c r="B139">
+        <v>6.7401821597361537E-4</v>
+      </c>
+      <c r="C139">
+        <v>1170</v>
+      </c>
+      <c r="D139">
+        <v>96.26</v>
+      </c>
+      <c r="E139">
+        <v>6.7401821597361537E-4</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G139" s="3">
+        <v>0.48569955749342414</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" s="1">
+        <v>40725</v>
+      </c>
+      <c r="B140">
+        <v>6.7182214943751302E-4</v>
+      </c>
+      <c r="C140">
+        <v>1510</v>
+      </c>
+      <c r="D140">
+        <v>97.3</v>
+      </c>
+      <c r="E140">
+        <v>6.7182214943751302E-4</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G140" s="3">
+        <v>223.92355360818934</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" ht="21" thickBot="1">
+      <c r="A141" s="1">
+        <v>40756</v>
+      </c>
+      <c r="B141">
+        <v>6.6721491839928464E-4</v>
+      </c>
+      <c r="C141">
+        <v>1380</v>
+      </c>
+      <c r="D141">
+        <v>86.33</v>
+      </c>
+      <c r="E141">
+        <v>6.6721491839928464E-4</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G141" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" s="1">
+        <v>40787</v>
+      </c>
+      <c r="B142">
+        <v>6.6509510510860573E-4</v>
+      </c>
+      <c r="C142">
+        <v>1350</v>
+      </c>
+      <c r="D142">
+        <v>85.52</v>
+      </c>
+      <c r="E142">
+        <v>6.6509510510860573E-4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" ht="21" thickBot="1">
+      <c r="A143" s="1">
+        <v>40817</v>
+      </c>
+      <c r="B143">
+        <v>6.6059571879100636E-4</v>
+      </c>
+      <c r="C143">
+        <v>1330</v>
+      </c>
+      <c r="D143">
+        <v>86.32</v>
+      </c>
+      <c r="E143">
+        <v>6.6059571879100636E-4</v>
+      </c>
+      <c r="F143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="1">
+        <v>40848</v>
+      </c>
+      <c r="B144">
+        <v>6.5735283596475374E-4</v>
+      </c>
+      <c r="C144">
+        <v>1320</v>
+      </c>
+      <c r="D144">
+        <v>97.16</v>
+      </c>
+      <c r="E144">
+        <v>6.5735283596475374E-4</v>
+      </c>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H144" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I144" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J144" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K144" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="1">
+        <v>40878</v>
+      </c>
+      <c r="B145">
+        <v>6.5415324433709763E-4</v>
+      </c>
+      <c r="C145">
+        <v>1420</v>
+      </c>
+      <c r="D145">
+        <v>98.56</v>
+      </c>
+      <c r="E145">
+        <v>6.5415324433709763E-4</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145" s="3">
+        <v>2</v>
+      </c>
+      <c r="H145" s="3">
+        <v>3462368.7076241449</v>
+      </c>
+      <c r="I145" s="3">
+        <v>1731184.3538120724</v>
+      </c>
+      <c r="J145" s="3">
+        <v>34.525801002584387</v>
+      </c>
+      <c r="K145" s="3">
+        <v>4.0631567805597279E-11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="1">
+        <v>40909</v>
+      </c>
+      <c r="B146">
+        <v>6.5222966297609703E-4</v>
+      </c>
+      <c r="C146">
+        <v>1250</v>
+      </c>
+      <c r="D146">
+        <v>100.27</v>
+      </c>
+      <c r="E146">
+        <v>6.5222966297609703E-4</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G146" s="3">
+        <v>69</v>
+      </c>
+      <c r="H146" s="3">
+        <v>3459781.2923758551</v>
+      </c>
+      <c r="I146" s="3">
+        <v>50141.75786051964</v>
+      </c>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+    </row>
+    <row r="147" spans="1:14" ht="21" thickBot="1">
+      <c r="A147" s="1">
+        <v>40940</v>
+      </c>
+      <c r="B147">
+        <v>6.5032426259012193E-4</v>
+      </c>
+      <c r="C147">
+        <v>1270</v>
+      </c>
+      <c r="D147">
+        <v>102.2</v>
+      </c>
+      <c r="E147">
+        <v>6.5032426259012193E-4</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G147" s="4">
+        <v>71</v>
+      </c>
+      <c r="H147" s="4">
+        <v>6922150</v>
+      </c>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+    </row>
+    <row r="148" spans="1:14" ht="21" thickBot="1">
+      <c r="A148" s="1">
+        <v>40969</v>
+      </c>
+      <c r="B148">
+        <v>6.4726549697252482E-4</v>
+      </c>
+      <c r="C148">
+        <v>1250</v>
+      </c>
+      <c r="D148">
+        <v>106.16</v>
+      </c>
+      <c r="E148">
+        <v>6.4726549697252482E-4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="1">
+        <v>41000</v>
+      </c>
+      <c r="B149">
+        <v>6.465669812529359E-4</v>
+      </c>
+      <c r="C149">
+        <v>1260</v>
+      </c>
+      <c r="D149">
+        <v>103.32</v>
+      </c>
+      <c r="E149">
+        <v>6.465669812529359E-4</v>
+      </c>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H149" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I149" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J149" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K149" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L149" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M149" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N149" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="1">
+        <v>41030</v>
+      </c>
+      <c r="B150">
+        <v>6.4355422845393249E-4</v>
+      </c>
+      <c r="C150">
+        <v>1380</v>
+      </c>
+      <c r="D150">
+        <v>94.66</v>
+      </c>
+      <c r="E150">
+        <v>6.4355422845393249E-4</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G150" s="3">
+        <v>-783.55100679903489</v>
+      </c>
+      <c r="H150" s="3">
+        <v>628.91595589897338</v>
+      </c>
+      <c r="I150" s="3">
+        <v>-1.2458755409997921</v>
+      </c>
+      <c r="J150" s="3">
+        <v>0.2170238729244163</v>
+      </c>
+      <c r="K150" s="3">
+        <v>-2038.2040095074763</v>
+      </c>
+      <c r="L150" s="3">
+        <v>471.10199590940647</v>
+      </c>
+      <c r="M150" s="3">
+        <v>-2038.2040095074763</v>
+      </c>
+      <c r="N150" s="3">
+        <v>471.10199590940647</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="1">
+        <v>41061</v>
+      </c>
+      <c r="B151">
+        <v>6.4287940504521661E-4</v>
+      </c>
+      <c r="C151">
+        <v>1250</v>
+      </c>
+      <c r="D151">
+        <v>82.3</v>
+      </c>
+      <c r="E151">
+        <v>6.4287940504521661E-4</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G151" s="3">
+        <v>5.5649483546605829</v>
+      </c>
+      <c r="H151" s="3">
+        <v>1.7588019951416838</v>
+      </c>
+      <c r="I151" s="3">
+        <v>3.164056198499074</v>
+      </c>
+      <c r="J151" s="3">
+        <v>2.3146089563615244E-3</v>
+      </c>
+      <c r="K151" s="3">
+        <v>2.0562343783712222</v>
+      </c>
+      <c r="L151" s="3">
+        <v>9.0736623309499436</v>
+      </c>
+      <c r="M151" s="3">
+        <v>2.0562343783712222</v>
+      </c>
+      <c r="N151" s="3">
+        <v>9.0736623309499436</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="21" thickBot="1">
+      <c r="A152" s="1">
+        <v>41091</v>
+      </c>
+      <c r="B152">
+        <v>6.3991149357519998E-4</v>
+      </c>
+      <c r="C152">
+        <v>1250</v>
+      </c>
+      <c r="D152">
+        <v>87.9</v>
+      </c>
+      <c r="E152">
+        <v>6.3991149357519998E-4</v>
+      </c>
+      <c r="F152" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G152" s="4">
+        <v>2588604.0816738065</v>
+      </c>
+      <c r="H152" s="4">
+        <v>1189847.1113432513</v>
+      </c>
+      <c r="I152" s="4">
+        <v>2.1755770611162468</v>
+      </c>
+      <c r="J152" s="4">
+        <v>3.3015189669754669E-2</v>
+      </c>
+      <c r="K152" s="4">
+        <v>214924.04222099902</v>
+      </c>
+      <c r="L152" s="4">
+        <v>4962284.1211266145</v>
+      </c>
+      <c r="M152" s="4">
+        <v>214924.04222099902</v>
+      </c>
+      <c r="N152" s="4">
+        <v>4962284.1211266145</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="1">
+        <v>41122</v>
+      </c>
+      <c r="B153">
+        <v>6.3925961203915242E-4</v>
+      </c>
+      <c r="C153">
+        <v>1180</v>
+      </c>
+      <c r="D153">
+        <v>94.13</v>
+      </c>
+      <c r="E153">
+        <v>6.3925961203915242E-4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="1">
+        <v>41153</v>
+      </c>
+      <c r="B154">
+        <v>6.3633541135295563E-4</v>
+      </c>
+      <c r="C154">
+        <v>1090</v>
+      </c>
+      <c r="D154">
+        <v>94.51</v>
+      </c>
+      <c r="E154">
+        <v>6.3633541135295563E-4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" ht="21" thickBot="1">
+      <c r="A155" s="1">
+        <v>41183</v>
+      </c>
+      <c r="B155">
+        <v>6.3570575031931793E-4</v>
+      </c>
+      <c r="C155">
+        <v>1110</v>
+      </c>
+      <c r="D155">
+        <v>89.49</v>
+      </c>
+      <c r="E155">
+        <v>6.3570575031931793E-4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="A156" s="1">
+        <v>41214</v>
+      </c>
+      <c r="B156">
+        <v>6.3282416901408456E-4</v>
+      </c>
+      <c r="C156">
+        <v>1120</v>
+      </c>
+      <c r="D156">
+        <v>86.53</v>
+      </c>
+      <c r="E156">
+        <v>6.3282416901408456E-4</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G156" s="6"/>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="A157" s="1">
+        <v>41244</v>
+      </c>
+      <c r="B157">
+        <v>6.3221603482341315E-4</v>
+      </c>
+      <c r="C157">
+        <v>1110</v>
+      </c>
+      <c r="D157">
+        <v>87.86</v>
+      </c>
+      <c r="E157">
+        <v>6.3221603482341315E-4</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G157" s="3">
+        <v>0.65396384365211424</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="A158" s="1">
+        <v>41275</v>
+      </c>
+      <c r="B158">
+        <v>6.2917620781295603E-4</v>
+      </c>
+      <c r="C158">
+        <v>1570</v>
+      </c>
+      <c r="D158">
+        <v>94.76</v>
+      </c>
+      <c r="E158">
+        <v>6.2917620781295603E-4</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G158" s="3">
+        <v>0.4276687088042469</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="A159" s="1">
+        <v>41306</v>
+      </c>
+      <c r="B159">
+        <v>6.2839140549355351E-4</v>
+      </c>
+      <c r="C159">
+        <v>1490</v>
+      </c>
+      <c r="D159">
+        <v>95.31</v>
+      </c>
+      <c r="E159">
+        <v>6.2839140549355351E-4</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G159" s="3">
+        <v>0.41949254750145043</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="1">
+        <v>41334</v>
+      </c>
+      <c r="B160">
+        <v>6.2761407827802542E-4</v>
+      </c>
+      <c r="C160">
+        <v>1510</v>
+      </c>
+      <c r="D160">
+        <v>92.94</v>
+      </c>
+      <c r="E160">
+        <v>6.2761407827802542E-4</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G160" s="3">
+        <v>237.90043077336495</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="21" thickBot="1">
+      <c r="A161" s="1">
+        <v>41365</v>
+      </c>
+      <c r="B161">
+        <v>6.2574170402002953E-4</v>
+      </c>
+      <c r="C161">
+        <v>1310</v>
+      </c>
+      <c r="D161">
+        <v>92.02</v>
+      </c>
+      <c r="E161">
+        <v>6.2574170402002953E-4</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G161" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="A162" s="1">
+        <v>41395</v>
+      </c>
+      <c r="B162">
+        <v>6.2608142599486559E-4</v>
+      </c>
+      <c r="C162">
+        <v>1060</v>
+      </c>
+      <c r="D162">
+        <v>94.51</v>
+      </c>
+      <c r="E162">
+        <v>6.2608142599486559E-4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="21" thickBot="1">
+      <c r="A163" s="1">
+        <v>41426</v>
+      </c>
+      <c r="B163">
+        <v>6.2532589431260187E-4</v>
+      </c>
+      <c r="C163">
+        <v>810</v>
+      </c>
+      <c r="D163">
+        <v>95.77</v>
+      </c>
+      <c r="E163">
+        <v>6.2532589431260187E-4</v>
+      </c>
+      <c r="F163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14">
+      <c r="A164" s="1">
+        <v>41456</v>
+      </c>
+      <c r="B164">
+        <v>6.2240350528804274E-4</v>
+      </c>
+      <c r="C164">
+        <v>1560</v>
+      </c>
+      <c r="D164">
+        <v>104.67</v>
+      </c>
+      <c r="E164">
+        <v>6.2240350528804274E-4</v>
+      </c>
+      <c r="F164" s="5"/>
+      <c r="G164" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H164" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I164" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K164" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14">
+      <c r="A165" s="1">
+        <v>41487</v>
+      </c>
+      <c r="B165">
+        <v>6.2167211092616808E-4</v>
+      </c>
+      <c r="C165">
+        <v>1670</v>
+      </c>
+      <c r="D165">
+        <v>106.57</v>
+      </c>
+      <c r="E165">
+        <v>6.2167211092616808E-4</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G165" s="3">
+        <v>1</v>
+      </c>
+      <c r="H165" s="3">
+        <v>2960386.9526493177</v>
+      </c>
+      <c r="I165" s="3">
+        <v>2960386.9526493177</v>
+      </c>
+      <c r="J165" s="3">
+        <v>52.306784683659849</v>
+      </c>
+      <c r="K165" s="3">
+        <v>4.701226727008321E-10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14">
+      <c r="A166" s="1">
+        <v>41518</v>
+      </c>
+      <c r="B166">
+        <v>6.209474894355606E-4</v>
+      </c>
+      <c r="C166">
+        <v>1360</v>
+      </c>
+      <c r="D166">
+        <v>106.29</v>
+      </c>
+      <c r="E166">
+        <v>6.209474894355606E-4</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G166" s="3">
+        <v>70</v>
+      </c>
+      <c r="H166" s="3">
+        <v>3961763.0473506823</v>
+      </c>
+      <c r="I166" s="3">
+        <v>56596.614962152606</v>
+      </c>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+    </row>
+    <row r="167" spans="1:14" ht="21" thickBot="1">
+      <c r="A167" s="1">
+        <v>41548</v>
+      </c>
+      <c r="B167">
+        <v>6.202295466815875E-4</v>
+      </c>
+      <c r="C167">
+        <v>1010</v>
+      </c>
+      <c r="D167">
+        <v>100.54</v>
+      </c>
+      <c r="E167">
+        <v>6.202295466815875E-4</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G167" s="4">
+        <v>71</v>
+      </c>
+      <c r="H167" s="4">
+        <v>6922150</v>
+      </c>
+      <c r="I167" s="4"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+    </row>
+    <row r="168" spans="1:14" ht="21" thickBot="1">
+      <c r="A168" s="1">
+        <v>41579</v>
+      </c>
+      <c r="B168">
+        <v>6.1951819172272949E-4</v>
+      </c>
+      <c r="C168">
+        <v>1390</v>
+      </c>
+      <c r="D168">
+        <v>93.86</v>
+      </c>
+      <c r="E168">
+        <v>6.1951819172272949E-4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="1">
+        <v>41609</v>
+      </c>
+      <c r="B169">
+        <v>6.1881333381966729E-4</v>
+      </c>
+      <c r="C169">
+        <v>1770</v>
+      </c>
+      <c r="D169">
+        <v>97.63</v>
+      </c>
+      <c r="E169">
+        <v>6.1881333381966729E-4</v>
+      </c>
+      <c r="F169" s="5"/>
+      <c r="G169" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J169" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K169" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L169" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M169" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N169" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="A170" s="1">
+        <v>41640</v>
+      </c>
+      <c r="B170">
+        <v>6.1791445607038806E-4</v>
+      </c>
+      <c r="C170">
+        <v>2000</v>
+      </c>
+      <c r="D170">
+        <v>94.62</v>
+      </c>
+      <c r="E170">
+        <v>6.1791445607038806E-4</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G170" s="3">
+        <v>-2182.7127596403466</v>
+      </c>
+      <c r="H170" s="3">
+        <v>475.11585626968753</v>
+      </c>
+      <c r="I170" s="3">
+        <v>-4.5940642284129218</v>
+      </c>
+      <c r="J170" s="3">
+        <v>1.8691760818643452E-5</v>
+      </c>
+      <c r="K170" s="3">
+        <v>-3130.301455775556</v>
+      </c>
+      <c r="L170" s="3">
+        <v>-1235.1240635051372</v>
+      </c>
+      <c r="M170" s="3">
+        <v>-3130.301455775556</v>
+      </c>
+      <c r="N170" s="3">
+        <v>-1235.1240635051372</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="21" thickBot="1">
+      <c r="A171" s="1">
+        <v>41671</v>
+      </c>
+      <c r="B171">
+        <v>6.1702428864529547E-4</v>
+      </c>
+      <c r="C171">
+        <v>1640</v>
+      </c>
+      <c r="D171">
+        <v>100.82</v>
+      </c>
+      <c r="E171">
+        <v>6.1702428864529547E-4</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G171" s="4">
+        <v>5573028.8864697851</v>
+      </c>
+      <c r="H171" s="4">
+        <v>770570.32799563068</v>
+      </c>
+      <c r="I171" s="4">
+        <v>7.2323429594882942</v>
+      </c>
+      <c r="J171" s="4">
+        <v>4.7012267270082538E-10</v>
+      </c>
+      <c r="K171" s="4">
+        <v>4036174.8270856044</v>
+      </c>
+      <c r="L171" s="4">
+        <v>7109882.9458539654</v>
+      </c>
+      <c r="M171" s="4">
+        <v>4036174.8270856044</v>
+      </c>
+      <c r="N171" s="4">
+        <v>7109882.9458539654</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14">
+      <c r="A172" s="1">
+        <v>41699</v>
+      </c>
+      <c r="B172">
+        <v>6.1404915259923888E-4</v>
+      </c>
+      <c r="C172">
+        <v>1210</v>
+      </c>
+      <c r="D172">
+        <v>100.8</v>
+      </c>
+      <c r="E172">
+        <v>6.1404915259923888E-4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14">
+      <c r="A173" s="1">
+        <v>41730</v>
+      </c>
+      <c r="B173">
+        <v>6.1214432323367226E-4</v>
+      </c>
+      <c r="C173">
+        <v>1390</v>
+      </c>
+      <c r="D173">
+        <v>102.07</v>
+      </c>
+      <c r="E173">
+        <v>6.1214432323367226E-4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14">
+      <c r="A174" s="1">
+        <v>41760</v>
+      </c>
+      <c r="B174">
+        <v>6.1025768715879428E-4</v>
+      </c>
+      <c r="C174">
+        <v>1580</v>
+      </c>
+      <c r="D174">
+        <v>102.18</v>
+      </c>
+      <c r="E174">
+        <v>6.1025768715879428E-4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14">
+      <c r="A175" s="1">
+        <v>41791</v>
+      </c>
+      <c r="B175">
+        <v>6.0735713516271695E-4</v>
+      </c>
+      <c r="C175">
+        <v>1540</v>
+      </c>
+      <c r="D175">
+        <v>105.79</v>
+      </c>
+      <c r="E175">
+        <v>6.0735713516271695E-4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14">
+      <c r="A176" s="1">
+        <v>41821</v>
+      </c>
+      <c r="B176">
+        <v>6.0448402535478844E-4</v>
+      </c>
+      <c r="C176">
+        <v>1570</v>
+      </c>
+      <c r="D176">
+        <v>103.59</v>
+      </c>
+      <c r="E176">
+        <v>6.0448402535478844E-4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1">
+        <v>41852</v>
+      </c>
+      <c r="B177">
+        <v>6.0368223833236602E-4</v>
+      </c>
+      <c r="C177">
+        <v>1540</v>
+      </c>
+      <c r="D177">
+        <v>96.54</v>
+      </c>
+      <c r="E177">
+        <v>6.0368223833236602E-4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B178">
+        <v>6.0085327752778628E-4</v>
+      </c>
+      <c r="C178">
+        <v>1280</v>
+      </c>
+      <c r="D178">
+        <v>93.21</v>
+      </c>
+      <c r="E178">
+        <v>6.0085327752778628E-4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B179">
+        <v>5.9805070706602371E-4</v>
+      </c>
+      <c r="C179">
+        <v>1070</v>
+      </c>
+      <c r="D179">
+        <v>84.4</v>
+      </c>
+      <c r="E179">
+        <v>5.9805070706602371E-4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="1">
+        <v>41944</v>
+      </c>
+      <c r="B180">
+        <v>5.9628205744718162E-4</v>
+      </c>
+      <c r="C180">
+        <v>1140</v>
+      </c>
+      <c r="D180">
+        <v>75.790000000000006</v>
+      </c>
+      <c r="E180">
+        <v>5.9628205744718162E-4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B181">
+        <v>5.9452975396431654E-4</v>
+      </c>
+      <c r="C181">
+        <v>1250</v>
+      </c>
+      <c r="D181">
+        <v>59.29</v>
+      </c>
+      <c r="E181">
+        <v>5.9452975396431654E-4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B182">
+        <v>5.9032653962288247E-4</v>
+      </c>
+      <c r="C182">
+        <v>1440</v>
+      </c>
+      <c r="D182" s="9">
+        <v>47.22</v>
+      </c>
+      <c r="E182">
+        <v>5.9032653962288247E-4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B183">
+        <v>5.8618233993985294E-4</v>
+      </c>
+      <c r="C183">
+        <v>1270</v>
+      </c>
+      <c r="D183" s="9">
+        <v>50.58</v>
+      </c>
+      <c r="E183">
+        <v>5.8618233993985294E-4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B184">
+        <v>5.8406043797393204E-4</v>
+      </c>
+      <c r="C184">
+        <v>1160</v>
+      </c>
+      <c r="D184" s="9">
+        <v>47.82</v>
+      </c>
+      <c r="E184">
+        <v>5.8406043797393204E-4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B185">
+        <v>5.8196791578082289E-4</v>
+      </c>
+      <c r="C185">
+        <v>890</v>
+      </c>
+      <c r="D185" s="9">
+        <v>54.45</v>
+      </c>
+      <c r="E185">
+        <v>5.8196791578082289E-4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B186">
+        <v>5.7990416736899064E-4</v>
+      </c>
+      <c r="C186">
+        <v>860</v>
+      </c>
+      <c r="D186" s="9">
+        <v>59.27</v>
+      </c>
+      <c r="E186">
+        <v>5.7990416736899064E-4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B187">
+        <v>5.7594432975611467E-4</v>
+      </c>
+      <c r="C187">
+        <v>720</v>
+      </c>
+      <c r="D187" s="9">
+        <v>59.82</v>
+      </c>
+      <c r="E187">
+        <v>5.7594432975611467E-4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="1">
+        <v>42186</v>
+      </c>
+      <c r="B188">
+        <v>5.7394942723875699E-4</v>
+      </c>
+      <c r="C188">
+        <v>900</v>
+      </c>
+      <c r="D188" s="9">
+        <v>50.9</v>
+      </c>
+      <c r="E188">
+        <v>5.7394942723875699E-4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="1">
+        <v>42217</v>
+      </c>
+      <c r="B189">
+        <v>5.7198140178711134E-4</v>
+      </c>
+      <c r="C189">
+        <v>1000</v>
+      </c>
+      <c r="D189" s="9">
+        <v>42.87</v>
+      </c>
+      <c r="E189">
+        <v>5.7198140178711134E-4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="1">
+        <v>42248</v>
+      </c>
+      <c r="B190">
+        <v>5.700397138688148E-4</v>
+      </c>
+      <c r="C190">
+        <v>910</v>
+      </c>
+      <c r="D190" s="9">
+        <v>45.48</v>
+      </c>
+      <c r="E190">
+        <v>5.700397138688148E-4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="1">
+        <v>42278</v>
+      </c>
+      <c r="B191">
+        <v>5.6625072644001504E-4</v>
+      </c>
+      <c r="C191">
+        <v>690</v>
+      </c>
+      <c r="D191" s="9">
+        <v>46.22</v>
+      </c>
+      <c r="E191">
+        <v>5.6625072644001504E-4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B192">
+        <v>5.643725200432816E-4</v>
+      </c>
+      <c r="C192">
+        <v>730</v>
+      </c>
+      <c r="D192" s="9">
+        <v>42.44</v>
+      </c>
+      <c r="E192">
+        <v>5.643725200432816E-4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B193">
+        <v>5.6251895451390652E-4</v>
+      </c>
+      <c r="C193">
+        <v>940</v>
+      </c>
+      <c r="D193" s="9">
+        <v>37.19</v>
+      </c>
+      <c r="E193">
+        <v>5.6251895451390652E-4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B194">
+        <v>5.6193868502046201E-4</v>
+      </c>
+      <c r="C194">
+        <v>990</v>
+      </c>
+      <c r="D194" s="9">
+        <v>31.68</v>
+      </c>
+      <c r="E194">
+        <v>5.6193868502046201E-4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B195">
+        <v>5.6320433947123908E-4</v>
+      </c>
+      <c r="C195">
+        <v>730</v>
+      </c>
+      <c r="D195" s="9">
+        <v>30.32</v>
+      </c>
+      <c r="E195">
+        <v>5.6320433947123908E-4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B196">
+        <v>5.6631021710881594E-4</v>
+      </c>
+      <c r="C196">
+        <v>640</v>
+      </c>
+      <c r="D196" s="9">
+        <v>37.549999999999997</v>
+      </c>
+      <c r="E196">
+        <v>5.6631021710881594E-4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B197">
+        <v>5.6756877286444026E-4</v>
+      </c>
+      <c r="C197">
+        <v>720</v>
+      </c>
+      <c r="D197" s="9">
+        <v>40.75</v>
+      </c>
+      <c r="E197">
+        <v>5.6756877286444026E-4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B198">
+        <v>5.6974426386877282E-4</v>
+      </c>
+      <c r="C198">
+        <v>880</v>
+      </c>
+      <c r="D198" s="9">
+        <v>46.71</v>
+      </c>
+      <c r="E198">
+        <v>5.6974426386877282E-4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B199">
+        <v>5.7191529004525646E-4</v>
+      </c>
+      <c r="C199">
+        <v>890</v>
+      </c>
+      <c r="D199" s="9">
+        <v>48.76</v>
+      </c>
+      <c r="E199">
+        <v>5.7191529004525646E-4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B200">
+        <v>5.7316422857142863E-4</v>
+      </c>
+      <c r="C200">
+        <v>1090</v>
+      </c>
+      <c r="D200" s="9">
+        <v>44.65</v>
+      </c>
+      <c r="E200">
+        <v>5.7316422857142863E-4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B201">
+        <v>5.7624400110810759E-4</v>
+      </c>
+      <c r="C201">
+        <v>1040</v>
+      </c>
+      <c r="D201" s="9">
+        <v>44.72</v>
+      </c>
+      <c r="E201">
+        <v>5.7624400110810759E-4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B202">
+        <v>5.7748595526818962E-4</v>
+      </c>
+      <c r="C202">
+        <v>1160</v>
+      </c>
+      <c r="D202" s="9">
+        <v>45.18</v>
+      </c>
+      <c r="E202">
+        <v>5.7748595526818962E-4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B203">
+        <v>5.7872537070857699E-4</v>
+      </c>
+      <c r="C203">
+        <v>1080</v>
+      </c>
+      <c r="D203" s="9">
+        <v>49.78</v>
+      </c>
+      <c r="E203">
+        <v>5.7872537070857699E-4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B204">
+        <v>5.81790031634976E-4</v>
+      </c>
+      <c r="C204">
+        <v>1170</v>
+      </c>
+      <c r="D204" s="9">
+        <v>45.66</v>
+      </c>
+      <c r="E204">
+        <v>5.81790031634976E-4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B205">
+        <v>5.8302252863472951E-4</v>
+      </c>
+      <c r="C205">
+        <v>1270</v>
+      </c>
+      <c r="D205" s="9">
+        <v>51.97</v>
+      </c>
+      <c r="E205">
+        <v>5.8302252863472951E-4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="D206" s="9">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="D207" s="9">
+        <v>53.47</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="D208" s="9">
+        <v>49.33</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4">
+      <c r="D209" s="9">
+        <v>51.06</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4">
+      <c r="D210" s="9">
+        <v>48.48</v>
+      </c>
+    </row>
+    <row r="211" spans="4:4">
+      <c r="D211" s="9">
+        <v>45.18</v>
+      </c>
+    </row>
+    <row r="212" spans="4:4">
+      <c r="D212" s="9">
+        <v>46.63</v>
+      </c>
+    </row>
+    <row r="213" spans="4:4">
+      <c r="D213" s="9">
+        <v>48.04</v>
+      </c>
+    </row>
+    <row r="214" spans="4:4">
+      <c r="D214" s="9">
+        <v>49.82</v>
+      </c>
+    </row>
+    <row r="215" spans="4:4">
+      <c r="D215" s="9">
+        <v>51.58</v>
+      </c>
+    </row>
+    <row r="216" spans="4:4">
+      <c r="D216" s="9">
+        <v>56.64</v>
+      </c>
+    </row>
+    <row r="217" spans="4:4">
+      <c r="D217" s="9">
+        <v>57.88</v>
+      </c>
+    </row>
+    <row r="218" spans="4:4">
+      <c r="D218" s="9">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="219" spans="4:4">
+      <c r="D219" s="9">
+        <v>62.23</v>
+      </c>
+    </row>
+    <row r="220" spans="4:4">
+      <c r="D220" s="9">
+        <v>62.73</v>
+      </c>
+    </row>
+    <row r="221" spans="4:4">
+      <c r="D221" s="9">
+        <v>66.25</v>
+      </c>
+    </row>
+    <row r="222" spans="4:4">
+      <c r="D222" s="9">
+        <v>69.98</v>
+      </c>
+    </row>
+    <row r="223" spans="4:4">
+      <c r="D223" s="9">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="224" spans="4:4">
+      <c r="D224" s="9">
+        <v>70.98</v>
+      </c>
+    </row>
+    <row r="225" spans="4:4">
+      <c r="D225" s="9">
+        <v>68.06</v>
+      </c>
+    </row>
+    <row r="226" spans="4:4">
+      <c r="D226" s="9">
+        <v>70.23</v>
+      </c>
+    </row>
+    <row r="227" spans="4:4">
+      <c r="D227" s="9">
+        <v>70.75</v>
+      </c>
+    </row>
+    <row r="228" spans="4:4">
+      <c r="D228" s="9">
+        <v>56.96</v>
+      </c>
+    </row>
+    <row r="229" spans="4:4">
+      <c r="D229" s="9">
+        <v>49.52</v>
+      </c>
+    </row>
+    <row r="230" spans="4:4">
+      <c r="D230" s="9">
+        <v>51.38</v>
+      </c>
+    </row>
+    <row r="231" spans="4:4">
+      <c r="D231" s="9">
+        <v>54.95</v>
+      </c>
+    </row>
+    <row r="232" spans="4:4">
+      <c r="D232" s="9">
+        <v>58.15</v>
+      </c>
+    </row>
+    <row r="233" spans="4:4">
+      <c r="D233" s="9">
+        <v>63.86</v>
+      </c>
+    </row>
+    <row r="234" spans="4:4">
+      <c r="D234" s="9">
+        <v>60.83</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1EF3A6-C6D7-6C40-A397-3F20CE72D830}">
   <dimension ref="A1:T216"/>
   <sheetViews>
@@ -21683,7 +24130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE618EF-1A9C-E843-879C-1D2485D28D0D}">
   <dimension ref="A1:S205"/>
   <sheetViews>
@@ -26183,7 +28630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662F7486-4381-4145-94DB-14583D06F1D7}">
   <dimension ref="A1:R214"/>
   <sheetViews>
@@ -29988,7 +32435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED6B15A-83EF-D046-9845-170FBB6FCCFF}">
   <dimension ref="A1:R214"/>
   <sheetViews>

</xml_diff>

<commit_message>
move data related file
</commit_message>
<xml_diff>
--- a/data/correlation/ship_demand_month.xlsx
+++ b/data/correlation/ship_demand_month.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8A4DA9-9BF9-314C-A9B1-5F4E34E8B731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC26DD45-EE67-5148-9781-D32527FEA0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
   </bookViews>
   <sheets>
     <sheet name="海事センター" sheetId="5" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="行き（原油追加）" sheetId="12" r:id="rId4"/>
     <sheet name="帰り（月）" sheetId="9" r:id="rId5"/>
     <sheet name="帰り（コンテナ積載数）" sheetId="11" r:id="rId6"/>
-    <sheet name="行き" sheetId="6" r:id="rId7"/>
-    <sheet name="帰り" sheetId="7" r:id="rId8"/>
+    <sheet name="帰り原油" sheetId="13" r:id="rId7"/>
+    <sheet name="行き" sheetId="6" r:id="rId8"/>
+    <sheet name="帰り" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="87">
   <si>
     <t>Gap</t>
     <phoneticPr fontId="1"/>
@@ -4527,7 +4528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF2D617-CD77-8E4D-948F-9B57BF5D174F}">
   <dimension ref="A1:Y214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:X1"/>
     </sheetView>
   </sheetViews>
@@ -13039,8 +13040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40FD581-74FB-F94A-9780-764D633DA0D6}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134:G205"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="107" workbookViewId="0">
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -17590,42 +17591,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="4:4">
+    <row r="209" spans="4:6">
       <c r="D209">
         <v>4</v>
       </c>
-    </row>
-    <row r="210" spans="4:4">
+      <c r="F209">
+        <f>AVERAGE(F134:F205)*3.894</f>
+        <v>2.3967664187903772E-3</v>
+      </c>
+    </row>
+    <row r="210" spans="4:6">
       <c r="D210">
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="4:4">
+    <row r="211" spans="4:6">
       <c r="D211">
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="4:4">
+    <row r="212" spans="4:6">
       <c r="D212">
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="4:4">
+    <row r="213" spans="4:6">
       <c r="D213">
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="4:4">
+    <row r="214" spans="4:6">
       <c r="D214">
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="4:4">
+    <row r="215" spans="4:6">
       <c r="D215">
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="4:4">
+    <row r="216" spans="4:6">
       <c r="D216">
         <v>11</v>
       </c>
@@ -17641,8 +17646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7311AD3-701D-CE48-8EB0-A330C275BCB3}">
   <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="H154" sqref="H154"/>
+    <sheetView topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="F208" sqref="F208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -19700,7 +19705,7 @@
         <v>5.643725200432816E-4</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:6">
       <c r="A193" s="1">
         <v>42339</v>
       </c>
@@ -19717,7 +19722,7 @@
         <v>5.6251895451390652E-4</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:6">
       <c r="A194" s="1">
         <v>42370</v>
       </c>
@@ -19734,7 +19739,7 @@
         <v>5.6193868502046201E-4</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:6">
       <c r="A195" s="1">
         <v>42401</v>
       </c>
@@ -19751,7 +19756,7 @@
         <v>5.6320433947123908E-4</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:6">
       <c r="A196" s="1">
         <v>42430</v>
       </c>
@@ -19768,7 +19773,7 @@
         <v>5.6631021710881594E-4</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:6">
       <c r="A197" s="1">
         <v>42461</v>
       </c>
@@ -19785,7 +19790,7 @@
         <v>5.6756877286444026E-4</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:6">
       <c r="A198" s="1">
         <v>42491</v>
       </c>
@@ -19802,7 +19807,7 @@
         <v>5.6974426386877282E-4</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:6">
       <c r="A199" s="1">
         <v>42522</v>
       </c>
@@ -19819,7 +19824,7 @@
         <v>5.7191529004525646E-4</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:6">
       <c r="A200" s="1">
         <v>42552</v>
       </c>
@@ -19836,7 +19841,7 @@
         <v>5.7316422857142863E-4</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:6">
       <c r="A201" s="1">
         <v>42583</v>
       </c>
@@ -19853,7 +19858,7 @@
         <v>5.7624400110810759E-4</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:6">
       <c r="A202" s="1">
         <v>42614</v>
       </c>
@@ -19870,7 +19875,7 @@
         <v>5.7748595526818962E-4</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:6">
       <c r="A203" s="1">
         <v>42644</v>
       </c>
@@ -19887,7 +19892,7 @@
         <v>5.7872537070857699E-4</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:6">
       <c r="A204" s="1">
         <v>42675</v>
       </c>
@@ -19904,7 +19909,7 @@
         <v>5.81790031634976E-4</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:6">
       <c r="A205" s="1">
         <v>42705</v>
       </c>
@@ -19921,17 +19926,21 @@
         <v>5.8302252863472951E-4</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:6">
       <c r="D206" s="9">
         <v>52.5</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:6">
       <c r="D207" s="9">
         <v>53.47</v>
       </c>
-    </row>
-    <row r="208" spans="1:5">
+      <c r="F207">
+        <f>AVERAGE(E134:E205)</f>
+        <v>6.1550241879567975E-4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
       <c r="D208" s="9">
         <v>49.33</v>
       </c>
@@ -24134,8 +24143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE618EF-1A9C-E843-879C-1D2485D28D0D}">
   <dimension ref="A1:S205"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G134" sqref="G134:G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -28631,6 +28640,2441 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E162AF47-0F82-E740-9473-AA0DA85EE082}">
+  <dimension ref="A1:N234"/>
+  <sheetViews>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="G150" sqref="G150"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1">
+        <v>36557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1">
+        <v>36586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1">
+        <v>36617</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1">
+        <v>36647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1">
+        <v>36678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1">
+        <v>36708</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1">
+        <v>36739</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1">
+        <v>36770</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1">
+        <v>36800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1">
+        <v>36831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1">
+        <v>36861</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1">
+        <v>36923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1">
+        <v>36951</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1">
+        <v>36982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1">
+        <v>37012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1">
+        <v>37043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1">
+        <v>37073</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1">
+        <v>37104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1">
+        <v>37135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1">
+        <v>37165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1">
+        <v>37196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1">
+        <v>37226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1">
+        <v>37288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1">
+        <v>37316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1">
+        <v>37347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1">
+        <v>37377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1">
+        <v>37408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1">
+        <v>37438</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1">
+        <v>37469</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1">
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1">
+        <v>37530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1">
+        <v>37561</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1">
+        <v>37591</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1">
+        <v>37622</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="1">
+        <v>37653</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="1">
+        <v>37681</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="1">
+        <v>37712</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1">
+        <v>37742</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1">
+        <v>37773</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1">
+        <v>37803</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1">
+        <v>37834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="1">
+        <v>37865</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1">
+        <v>37895</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="1">
+        <v>37926</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1">
+        <v>37956</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1">
+        <v>38018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="1">
+        <v>38047</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="1">
+        <v>38078</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="1">
+        <v>38108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="1">
+        <v>38139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="1">
+        <v>38169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="1">
+        <v>38200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="1">
+        <v>38231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="1">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="1">
+        <v>38292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="1">
+        <v>38322</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="1">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="1">
+        <v>38384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="1">
+        <v>38412</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1">
+        <v>38443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="1">
+        <v>38473</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="1">
+        <v>38504</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="1">
+        <v>38534</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="1">
+        <v>38565</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="1">
+        <v>38596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="1">
+        <v>38626</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="1">
+        <v>38657</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="1">
+        <v>38687</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="1">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="1">
+        <v>38749</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="1">
+        <v>38777</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="1">
+        <v>38808</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="1">
+        <v>38838</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="1">
+        <v>38869</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="1">
+        <v>38899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="1">
+        <v>38930</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="1">
+        <v>38961</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="1">
+        <v>38991</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="1">
+        <v>39022</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="1">
+        <v>39052</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="1">
+        <v>39083</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="1">
+        <v>39114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1">
+        <v>39142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="1">
+        <v>39173</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="1">
+        <v>39203</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="1">
+        <v>39234</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="1">
+        <v>39264</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="1">
+        <v>39295</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="1">
+        <v>39326</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="1">
+        <v>39356</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="1">
+        <v>39387</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="1">
+        <v>39417</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1">
+        <v>39479</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="1">
+        <v>39508</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="1">
+        <v>39539</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="1">
+        <v>39569</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="1">
+        <v>39600</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="1">
+        <v>39630</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="1">
+        <v>39661</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1">
+        <v>39692</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1">
+        <v>39722</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="1">
+        <v>39753</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="1">
+        <v>39783</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1">
+        <v>39814</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="1">
+        <v>39845</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1">
+        <v>39873</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1">
+        <v>39904</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1">
+        <v>39934</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1">
+        <v>39965</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1">
+        <v>39995</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="1">
+        <v>40026</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1">
+        <v>40057</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="1">
+        <v>40087</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="1">
+        <v>40118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1">
+        <v>40148</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="1">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1">
+        <v>40210</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="1">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="1">
+        <v>40269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1">
+        <v>40299</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="1">
+        <v>40330</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="1">
+        <v>40360</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="1">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="1">
+        <v>40422</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="1">
+        <v>40452</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1">
+        <v>40483</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="1">
+        <v>40513</v>
+      </c>
+      <c r="F133" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="1">
+        <v>40544</v>
+      </c>
+      <c r="B134">
+        <v>6.9188410682729498E-4</v>
+      </c>
+      <c r="C134" s="8">
+        <v>830</v>
+      </c>
+      <c r="D134">
+        <v>89.17</v>
+      </c>
+      <c r="E134">
+        <v>6.9188410682729498E-4</v>
+      </c>
+      <c r="F134" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="21" thickBot="1">
+      <c r="A135" s="1">
+        <v>40575</v>
+      </c>
+      <c r="B135">
+        <v>6.8820870551067283E-4</v>
+      </c>
+      <c r="C135" s="8">
+        <v>850</v>
+      </c>
+      <c r="D135">
+        <v>88.58</v>
+      </c>
+      <c r="E135">
+        <v>6.8820870551067283E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="A136" s="1">
+        <v>40603</v>
+      </c>
+      <c r="B136">
+        <v>6.8584948809213755E-4</v>
+      </c>
+      <c r="C136" s="8">
+        <v>750</v>
+      </c>
+      <c r="D136">
+        <v>102.86</v>
+      </c>
+      <c r="E136">
+        <v>6.8584948809213755E-4</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" s="6"/>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="A137" s="1">
+        <v>40634</v>
+      </c>
+      <c r="B137">
+        <v>6.8101340022527182E-4</v>
+      </c>
+      <c r="C137" s="8">
+        <v>740</v>
+      </c>
+      <c r="D137">
+        <v>109.53</v>
+      </c>
+      <c r="E137">
+        <v>6.8101340022527182E-4</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G137" s="3">
+        <v>0.5878680285601503</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="A138" s="1">
+        <v>40664</v>
+      </c>
+      <c r="B138">
+        <v>6.787376012189068E-4</v>
+      </c>
+      <c r="C138" s="8">
+        <v>670</v>
+      </c>
+      <c r="D138">
+        <v>100.9</v>
+      </c>
+      <c r="E138">
+        <v>6.787376012189068E-4</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G138" s="3">
+        <v>0.34558881900319766</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" s="1">
+        <v>40695</v>
+      </c>
+      <c r="B139">
+        <v>6.7401821597361537E-4</v>
+      </c>
+      <c r="C139" s="8">
+        <v>680</v>
+      </c>
+      <c r="D139">
+        <v>96.26</v>
+      </c>
+      <c r="E139">
+        <v>6.7401821597361537E-4</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G139" s="3">
+        <v>0.32662037897430485</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" s="1">
+        <v>40725</v>
+      </c>
+      <c r="B140">
+        <v>6.7182214943751302E-4</v>
+      </c>
+      <c r="C140" s="8">
+        <v>870</v>
+      </c>
+      <c r="D140">
+        <v>97.3</v>
+      </c>
+      <c r="E140">
+        <v>6.7182214943751302E-4</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G140" s="3">
+        <v>119.78002265342</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" ht="21" thickBot="1">
+      <c r="A141" s="1">
+        <v>40756</v>
+      </c>
+      <c r="B141">
+        <v>6.6721491839928464E-4</v>
+      </c>
+      <c r="C141" s="8">
+        <v>800</v>
+      </c>
+      <c r="D141">
+        <v>86.33</v>
+      </c>
+      <c r="E141">
+        <v>6.6721491839928464E-4</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G141" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" s="1">
+        <v>40787</v>
+      </c>
+      <c r="B142">
+        <v>6.6509510510860573E-4</v>
+      </c>
+      <c r="C142" s="8">
+        <v>820</v>
+      </c>
+      <c r="D142">
+        <v>85.52</v>
+      </c>
+      <c r="E142">
+        <v>6.6509510510860573E-4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" ht="21" thickBot="1">
+      <c r="A143" s="1">
+        <v>40817</v>
+      </c>
+      <c r="B143">
+        <v>6.6059571879100636E-4</v>
+      </c>
+      <c r="C143" s="8">
+        <v>690</v>
+      </c>
+      <c r="D143">
+        <v>86.32</v>
+      </c>
+      <c r="E143">
+        <v>6.6059571879100636E-4</v>
+      </c>
+      <c r="F143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="1">
+        <v>40848</v>
+      </c>
+      <c r="B144">
+        <v>6.5735283596475374E-4</v>
+      </c>
+      <c r="C144" s="8">
+        <v>750</v>
+      </c>
+      <c r="D144">
+        <v>97.16</v>
+      </c>
+      <c r="E144">
+        <v>6.5735283596475374E-4</v>
+      </c>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H144" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I144" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J144" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K144" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="A145" s="1">
+        <v>40878</v>
+      </c>
+      <c r="B145">
+        <v>6.5415324433709763E-4</v>
+      </c>
+      <c r="C145" s="8">
+        <v>820</v>
+      </c>
+      <c r="D145">
+        <v>98.56</v>
+      </c>
+      <c r="E145">
+        <v>6.5415324433709763E-4</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145" s="3">
+        <v>2</v>
+      </c>
+      <c r="H145" s="3">
+        <v>522789.48594708729</v>
+      </c>
+      <c r="I145" s="3">
+        <v>261394.74297354365</v>
+      </c>
+      <c r="J145" s="3">
+        <v>18.219148146963857</v>
+      </c>
+      <c r="K145" s="3">
+        <v>4.4345496948696161E-7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="1">
+        <v>40909</v>
+      </c>
+      <c r="B146">
+        <v>6.5222966297609703E-4</v>
+      </c>
+      <c r="C146" s="8">
+        <v>730</v>
+      </c>
+      <c r="D146">
+        <v>100.27</v>
+      </c>
+      <c r="E146">
+        <v>6.5222966297609703E-4</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G146" s="3">
+        <v>69</v>
+      </c>
+      <c r="H146" s="3">
+        <v>989960.51405291271</v>
+      </c>
+      <c r="I146" s="3">
+        <v>14347.253826853808</v>
+      </c>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+    </row>
+    <row r="147" spans="1:14" ht="21" thickBot="1">
+      <c r="A147" s="1">
+        <v>40940</v>
+      </c>
+      <c r="B147">
+        <v>6.5032426259012193E-4</v>
+      </c>
+      <c r="C147" s="8">
+        <v>650</v>
+      </c>
+      <c r="D147">
+        <v>102.2</v>
+      </c>
+      <c r="E147">
+        <v>6.5032426259012193E-4</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G147" s="4">
+        <v>71</v>
+      </c>
+      <c r="H147" s="4">
+        <v>1512750</v>
+      </c>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+    </row>
+    <row r="148" spans="1:14" ht="21" thickBot="1">
+      <c r="A148" s="1">
+        <v>40969</v>
+      </c>
+      <c r="B148">
+        <v>6.4726549697252482E-4</v>
+      </c>
+      <c r="C148" s="8">
+        <v>850</v>
+      </c>
+      <c r="D148">
+        <v>106.16</v>
+      </c>
+      <c r="E148">
+        <v>6.4726549697252482E-4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="A149" s="1">
+        <v>41000</v>
+      </c>
+      <c r="B149">
+        <v>6.465669812529359E-4</v>
+      </c>
+      <c r="C149" s="8">
+        <v>900</v>
+      </c>
+      <c r="D149">
+        <v>103.32</v>
+      </c>
+      <c r="E149">
+        <v>6.465669812529359E-4</v>
+      </c>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H149" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I149" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J149" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K149" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L149" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M149" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N149" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="1">
+        <v>41030</v>
+      </c>
+      <c r="B150">
+        <v>6.4355422845393249E-4</v>
+      </c>
+      <c r="C150" s="8">
+        <v>1080</v>
+      </c>
+      <c r="D150">
+        <v>94.66</v>
+      </c>
+      <c r="E150">
+        <v>6.4355422845393249E-4</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G150" s="3">
+        <v>479.75714148843963</v>
+      </c>
+      <c r="H150" s="3">
+        <v>336.41645209189505</v>
+      </c>
+      <c r="I150" s="3">
+        <v>1.4260810923640257</v>
+      </c>
+      <c r="J150" s="3">
+        <v>0.15835375578260072</v>
+      </c>
+      <c r="K150" s="3">
+        <v>-191.37531717892944</v>
+      </c>
+      <c r="L150" s="3">
+        <v>1150.8896001558087</v>
+      </c>
+      <c r="M150" s="3">
+        <v>-191.37531717892944</v>
+      </c>
+      <c r="N150" s="3">
+        <v>1150.8896001558087</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="1">
+        <v>41061</v>
+      </c>
+      <c r="B151">
+        <v>6.4287940504521661E-4</v>
+      </c>
+      <c r="C151" s="8">
+        <v>1180</v>
+      </c>
+      <c r="D151">
+        <v>82.3</v>
+      </c>
+      <c r="E151">
+        <v>6.4287940504521661E-4</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G151" s="3">
+        <v>3.3552750205878263</v>
+      </c>
+      <c r="H151" s="3">
+        <v>0.94080921558421782</v>
+      </c>
+      <c r="I151" s="3">
+        <v>3.5663713375769697</v>
+      </c>
+      <c r="J151" s="3">
+        <v>6.6295417612866243E-4</v>
+      </c>
+      <c r="K151" s="3">
+        <v>1.4784119894674561</v>
+      </c>
+      <c r="L151" s="3">
+        <v>5.2321380517081968</v>
+      </c>
+      <c r="M151" s="3">
+        <v>1.4784119894674561</v>
+      </c>
+      <c r="N151" s="3">
+        <v>5.2321380517081968</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="21" thickBot="1">
+      <c r="A152" s="1">
+        <v>41091</v>
+      </c>
+      <c r="B152">
+        <v>6.3991149357519998E-4</v>
+      </c>
+      <c r="C152" s="8">
+        <v>1160</v>
+      </c>
+      <c r="D152">
+        <v>87.9</v>
+      </c>
+      <c r="E152">
+        <v>6.3991149357519998E-4</v>
+      </c>
+      <c r="F152" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G152" s="4">
+        <v>90123.895689019468</v>
+      </c>
+      <c r="H152" s="4">
+        <v>636466.82831845153</v>
+      </c>
+      <c r="I152" s="4">
+        <v>0.14160030292093501</v>
+      </c>
+      <c r="J152" s="4">
+        <v>0.88780834779873374</v>
+      </c>
+      <c r="K152" s="4">
+        <v>-1179592.6853327195</v>
+      </c>
+      <c r="L152" s="4">
+        <v>1359840.4767107584</v>
+      </c>
+      <c r="M152" s="4">
+        <v>-1179592.6853327195</v>
+      </c>
+      <c r="N152" s="4">
+        <v>1359840.4767107584</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="1">
+        <v>41122</v>
+      </c>
+      <c r="B153">
+        <v>6.3925961203915242E-4</v>
+      </c>
+      <c r="C153" s="8">
+        <v>1150</v>
+      </c>
+      <c r="D153">
+        <v>94.13</v>
+      </c>
+      <c r="E153">
+        <v>6.3925961203915242E-4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="1">
+        <v>41153</v>
+      </c>
+      <c r="B154">
+        <v>6.3633541135295563E-4</v>
+      </c>
+      <c r="C154" s="8">
+        <v>1010</v>
+      </c>
+      <c r="D154">
+        <v>94.51</v>
+      </c>
+      <c r="E154">
+        <v>6.3633541135295563E-4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" ht="21" thickBot="1">
+      <c r="A155" s="1">
+        <v>41183</v>
+      </c>
+      <c r="B155">
+        <v>6.3570575031931793E-4</v>
+      </c>
+      <c r="C155" s="8">
+        <v>1090</v>
+      </c>
+      <c r="D155">
+        <v>89.49</v>
+      </c>
+      <c r="E155">
+        <v>6.3570575031931793E-4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="A156" s="1">
+        <v>41214</v>
+      </c>
+      <c r="B156">
+        <v>6.3282416901408456E-4</v>
+      </c>
+      <c r="C156" s="8">
+        <v>1040</v>
+      </c>
+      <c r="D156">
+        <v>86.53</v>
+      </c>
+      <c r="E156">
+        <v>6.3282416901408456E-4</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G156" s="6"/>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="A157" s="1">
+        <v>41244</v>
+      </c>
+      <c r="B157">
+        <v>6.3221603482341315E-4</v>
+      </c>
+      <c r="C157" s="8">
+        <v>1080</v>
+      </c>
+      <c r="D157">
+        <v>87.86</v>
+      </c>
+      <c r="E157">
+        <v>6.3221603482341315E-4</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G157" s="3">
+        <v>0.47429841006963136</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="A158" s="1">
+        <v>41275</v>
+      </c>
+      <c r="B158">
+        <v>6.2917620781295603E-4</v>
+      </c>
+      <c r="C158" s="8">
+        <v>970</v>
+      </c>
+      <c r="D158">
+        <v>94.76</v>
+      </c>
+      <c r="E158">
+        <v>6.2917620781295603E-4</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G158" s="3">
+        <v>0.22495898179458018</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="A159" s="1">
+        <v>41306</v>
+      </c>
+      <c r="B159">
+        <v>6.2839140549355351E-4</v>
+      </c>
+      <c r="C159" s="8">
+        <v>950</v>
+      </c>
+      <c r="D159">
+        <v>95.31</v>
+      </c>
+      <c r="E159">
+        <v>6.2839140549355351E-4</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G159" s="3">
+        <v>0.21388696724878847</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="1">
+        <v>41334</v>
+      </c>
+      <c r="B160">
+        <v>6.2761407827802542E-4</v>
+      </c>
+      <c r="C160" s="8">
+        <v>910</v>
+      </c>
+      <c r="D160">
+        <v>92.94</v>
+      </c>
+      <c r="E160">
+        <v>6.2761407827802542E-4</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G160" s="3">
+        <v>129.41866173062681</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="21" thickBot="1">
+      <c r="A161" s="1">
+        <v>41365</v>
+      </c>
+      <c r="B161">
+        <v>6.2574170402002953E-4</v>
+      </c>
+      <c r="C161" s="8">
+        <v>920</v>
+      </c>
+      <c r="D161">
+        <v>92.02</v>
+      </c>
+      <c r="E161">
+        <v>6.2574170402002953E-4</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G161" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="A162" s="1">
+        <v>41395</v>
+      </c>
+      <c r="B162">
+        <v>6.2608142599486559E-4</v>
+      </c>
+      <c r="C162" s="8">
+        <v>800</v>
+      </c>
+      <c r="D162">
+        <v>94.51</v>
+      </c>
+      <c r="E162">
+        <v>6.2608142599486559E-4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="21" thickBot="1">
+      <c r="A163" s="1">
+        <v>41426</v>
+      </c>
+      <c r="B163">
+        <v>6.2532589431260187E-4</v>
+      </c>
+      <c r="C163" s="8">
+        <v>820</v>
+      </c>
+      <c r="D163">
+        <v>95.77</v>
+      </c>
+      <c r="E163">
+        <v>6.2532589431260187E-4</v>
+      </c>
+      <c r="F163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14">
+      <c r="A164" s="1">
+        <v>41456</v>
+      </c>
+      <c r="B164">
+        <v>6.2240350528804274E-4</v>
+      </c>
+      <c r="C164" s="8">
+        <v>830</v>
+      </c>
+      <c r="D164">
+        <v>104.67</v>
+      </c>
+      <c r="E164">
+        <v>6.2240350528804274E-4</v>
+      </c>
+      <c r="F164" s="5"/>
+      <c r="G164" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H164" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I164" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K164" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14">
+      <c r="A165" s="1">
+        <v>41487</v>
+      </c>
+      <c r="B165">
+        <v>6.2167211092616808E-4</v>
+      </c>
+      <c r="C165" s="8">
+        <v>850</v>
+      </c>
+      <c r="D165">
+        <v>106.57</v>
+      </c>
+      <c r="E165">
+        <v>6.2167211092616808E-4</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G165" s="3">
+        <v>1</v>
+      </c>
+      <c r="H165" s="3">
+        <v>340306.69970975118</v>
+      </c>
+      <c r="I165" s="3">
+        <v>340306.69970975118</v>
+      </c>
+      <c r="J165" s="3">
+        <v>20.317800420528112</v>
+      </c>
+      <c r="K165" s="3">
+        <v>2.5666335851840877E-5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14">
+      <c r="A166" s="1">
+        <v>41518</v>
+      </c>
+      <c r="B166">
+        <v>6.209474894355606E-4</v>
+      </c>
+      <c r="C166" s="8">
+        <v>860</v>
+      </c>
+      <c r="D166">
+        <v>106.29</v>
+      </c>
+      <c r="E166">
+        <v>6.209474894355606E-4</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G166" s="3">
+        <v>70</v>
+      </c>
+      <c r="H166" s="3">
+        <v>1172443.3002902488</v>
+      </c>
+      <c r="I166" s="3">
+        <v>16749.190004146411</v>
+      </c>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+    </row>
+    <row r="167" spans="1:14" ht="21" thickBot="1">
+      <c r="A167" s="1">
+        <v>41548</v>
+      </c>
+      <c r="B167">
+        <v>6.202295466815875E-4</v>
+      </c>
+      <c r="C167" s="8">
+        <v>820</v>
+      </c>
+      <c r="D167">
+        <v>100.54</v>
+      </c>
+      <c r="E167">
+        <v>6.202295466815875E-4</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G167" s="4">
+        <v>71</v>
+      </c>
+      <c r="H167" s="4">
+        <v>1512750</v>
+      </c>
+      <c r="I167" s="4"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+    </row>
+    <row r="168" spans="1:14" ht="21" thickBot="1">
+      <c r="A168" s="1">
+        <v>41579</v>
+      </c>
+      <c r="B168">
+        <v>6.1951819172272949E-4</v>
+      </c>
+      <c r="C168" s="8">
+        <v>800</v>
+      </c>
+      <c r="D168">
+        <v>93.86</v>
+      </c>
+      <c r="E168">
+        <v>6.1951819172272949E-4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="1">
+        <v>41609</v>
+      </c>
+      <c r="B169">
+        <v>6.1881333381966729E-4</v>
+      </c>
+      <c r="C169" s="8">
+        <v>800</v>
+      </c>
+      <c r="D169">
+        <v>97.63</v>
+      </c>
+      <c r="E169">
+        <v>6.1881333381966729E-4</v>
+      </c>
+      <c r="F169" s="5"/>
+      <c r="G169" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J169" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K169" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L169" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M169" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N169" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="A170" s="1">
+        <v>41640</v>
+      </c>
+      <c r="B170">
+        <v>6.1791445607038806E-4</v>
+      </c>
+      <c r="C170" s="8">
+        <v>820</v>
+      </c>
+      <c r="D170">
+        <v>94.62</v>
+      </c>
+      <c r="E170">
+        <v>6.1791445607038806E-4</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G170" s="3">
+        <v>-363.83963244005088</v>
+      </c>
+      <c r="H170" s="3">
+        <v>258.46467820817423</v>
+      </c>
+      <c r="I170" s="3">
+        <v>-1.4076957631595792</v>
+      </c>
+      <c r="J170" s="3">
+        <v>0.1636465656632996</v>
+      </c>
+      <c r="K170" s="3">
+        <v>-879.3311787404308</v>
+      </c>
+      <c r="L170" s="3">
+        <v>151.65191386032905</v>
+      </c>
+      <c r="M170" s="3">
+        <v>-879.3311787404308</v>
+      </c>
+      <c r="N170" s="3">
+        <v>151.65191386032905</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="21" thickBot="1">
+      <c r="A171" s="1">
+        <v>41671</v>
+      </c>
+      <c r="B171">
+        <v>6.1702428864529547E-4</v>
+      </c>
+      <c r="C171" s="8">
+        <v>820</v>
+      </c>
+      <c r="D171">
+        <v>100.82</v>
+      </c>
+      <c r="E171">
+        <v>6.1702428864529547E-4</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G171" s="4">
+        <v>1889523.5235343331</v>
+      </c>
+      <c r="H171" s="4">
+        <v>419192.93838323693</v>
+      </c>
+      <c r="I171" s="4">
+        <v>4.5075270848357709</v>
+      </c>
+      <c r="J171" s="4">
+        <v>2.5666335851841608E-5</v>
+      </c>
+      <c r="K171" s="4">
+        <v>1053469.5702303937</v>
+      </c>
+      <c r="L171" s="4">
+        <v>2725577.4768382725</v>
+      </c>
+      <c r="M171" s="4">
+        <v>1053469.5702303937</v>
+      </c>
+      <c r="N171" s="4">
+        <v>2725577.4768382725</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14">
+      <c r="A172" s="1">
+        <v>41699</v>
+      </c>
+      <c r="B172">
+        <v>6.1404915259923888E-4</v>
+      </c>
+      <c r="C172" s="8">
+        <v>890</v>
+      </c>
+      <c r="D172">
+        <v>100.8</v>
+      </c>
+      <c r="E172">
+        <v>6.1404915259923888E-4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14">
+      <c r="A173" s="1">
+        <v>41730</v>
+      </c>
+      <c r="B173">
+        <v>6.1214432323367226E-4</v>
+      </c>
+      <c r="C173" s="8">
+        <v>850</v>
+      </c>
+      <c r="D173">
+        <v>102.07</v>
+      </c>
+      <c r="E173">
+        <v>6.1214432323367226E-4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14">
+      <c r="A174" s="1">
+        <v>41760</v>
+      </c>
+      <c r="B174">
+        <v>6.1025768715879428E-4</v>
+      </c>
+      <c r="C174" s="8">
+        <v>860</v>
+      </c>
+      <c r="D174">
+        <v>102.18</v>
+      </c>
+      <c r="E174">
+        <v>6.1025768715879428E-4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14">
+      <c r="A175" s="1">
+        <v>41791</v>
+      </c>
+      <c r="B175">
+        <v>6.0735713516271695E-4</v>
+      </c>
+      <c r="C175" s="8">
+        <v>850</v>
+      </c>
+      <c r="D175">
+        <v>105.79</v>
+      </c>
+      <c r="E175">
+        <v>6.0735713516271695E-4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14">
+      <c r="A176" s="1">
+        <v>41821</v>
+      </c>
+      <c r="B176">
+        <v>6.0448402535478844E-4</v>
+      </c>
+      <c r="C176" s="8">
+        <v>840</v>
+      </c>
+      <c r="D176">
+        <v>103.59</v>
+      </c>
+      <c r="E176">
+        <v>6.0448402535478844E-4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1">
+        <v>41852</v>
+      </c>
+      <c r="B177">
+        <v>6.0368223833236602E-4</v>
+      </c>
+      <c r="C177" s="8">
+        <v>840</v>
+      </c>
+      <c r="D177">
+        <v>96.54</v>
+      </c>
+      <c r="E177">
+        <v>6.0368223833236602E-4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B178">
+        <v>6.0085327752778628E-4</v>
+      </c>
+      <c r="C178" s="8">
+        <v>810</v>
+      </c>
+      <c r="D178">
+        <v>93.21</v>
+      </c>
+      <c r="E178">
+        <v>6.0085327752778628E-4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B179">
+        <v>5.9805070706602371E-4</v>
+      </c>
+      <c r="C179" s="8">
+        <v>850</v>
+      </c>
+      <c r="D179">
+        <v>84.4</v>
+      </c>
+      <c r="E179">
+        <v>5.9805070706602371E-4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="1">
+        <v>41944</v>
+      </c>
+      <c r="B180">
+        <v>5.9628205744718162E-4</v>
+      </c>
+      <c r="C180" s="8">
+        <v>860</v>
+      </c>
+      <c r="D180">
+        <v>75.790000000000006</v>
+      </c>
+      <c r="E180">
+        <v>5.9628205744718162E-4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B181">
+        <v>5.9452975396431654E-4</v>
+      </c>
+      <c r="C181" s="8">
+        <v>810</v>
+      </c>
+      <c r="D181">
+        <v>59.29</v>
+      </c>
+      <c r="E181">
+        <v>5.9452975396431654E-4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B182">
+        <v>5.9032653962288247E-4</v>
+      </c>
+      <c r="C182" s="8">
+        <v>790</v>
+      </c>
+      <c r="D182" s="9">
+        <v>47.22</v>
+      </c>
+      <c r="E182">
+        <v>5.9032653962288247E-4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B183">
+        <v>5.8618233993985294E-4</v>
+      </c>
+      <c r="C183" s="8">
+        <v>700</v>
+      </c>
+      <c r="D183" s="9">
+        <v>50.58</v>
+      </c>
+      <c r="E183">
+        <v>5.8618233993985294E-4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B184">
+        <v>5.8406043797393204E-4</v>
+      </c>
+      <c r="C184" s="8">
+        <v>830</v>
+      </c>
+      <c r="D184" s="9">
+        <v>47.82</v>
+      </c>
+      <c r="E184">
+        <v>5.8406043797393204E-4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B185">
+        <v>5.8196791578082289E-4</v>
+      </c>
+      <c r="C185" s="8">
+        <v>780</v>
+      </c>
+      <c r="D185" s="9">
+        <v>54.45</v>
+      </c>
+      <c r="E185">
+        <v>5.8196791578082289E-4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B186">
+        <v>5.7990416736899064E-4</v>
+      </c>
+      <c r="C186" s="8">
+        <v>770</v>
+      </c>
+      <c r="D186" s="9">
+        <v>59.27</v>
+      </c>
+      <c r="E186">
+        <v>5.7990416736899064E-4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B187">
+        <v>5.7594432975611467E-4</v>
+      </c>
+      <c r="C187" s="8">
+        <v>710</v>
+      </c>
+      <c r="D187" s="9">
+        <v>59.82</v>
+      </c>
+      <c r="E187">
+        <v>5.7594432975611467E-4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="1">
+        <v>42186</v>
+      </c>
+      <c r="B188">
+        <v>5.7394942723875699E-4</v>
+      </c>
+      <c r="C188" s="8">
+        <v>680</v>
+      </c>
+      <c r="D188" s="9">
+        <v>50.9</v>
+      </c>
+      <c r="E188">
+        <v>5.7394942723875699E-4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="1">
+        <v>42217</v>
+      </c>
+      <c r="B189">
+        <v>5.7198140178711134E-4</v>
+      </c>
+      <c r="C189" s="8">
+        <v>640</v>
+      </c>
+      <c r="D189" s="9">
+        <v>42.87</v>
+      </c>
+      <c r="E189">
+        <v>5.7198140178711134E-4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="1">
+        <v>42248</v>
+      </c>
+      <c r="B190">
+        <v>5.700397138688148E-4</v>
+      </c>
+      <c r="C190" s="8">
+        <v>660</v>
+      </c>
+      <c r="D190" s="9">
+        <v>45.48</v>
+      </c>
+      <c r="E190">
+        <v>5.700397138688148E-4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="1">
+        <v>42278</v>
+      </c>
+      <c r="B191">
+        <v>5.6625072644001504E-4</v>
+      </c>
+      <c r="C191" s="8">
+        <v>640</v>
+      </c>
+      <c r="D191" s="9">
+        <v>46.22</v>
+      </c>
+      <c r="E191">
+        <v>5.6625072644001504E-4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B192">
+        <v>5.643725200432816E-4</v>
+      </c>
+      <c r="C192" s="8">
+        <v>650</v>
+      </c>
+      <c r="D192" s="9">
+        <v>42.44</v>
+      </c>
+      <c r="E192">
+        <v>5.643725200432816E-4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B193">
+        <v>5.6251895451390652E-4</v>
+      </c>
+      <c r="C193" s="8">
+        <v>610</v>
+      </c>
+      <c r="D193" s="9">
+        <v>37.19</v>
+      </c>
+      <c r="E193">
+        <v>5.6251895451390652E-4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B194">
+        <v>5.6193868502046201E-4</v>
+      </c>
+      <c r="C194" s="8">
+        <v>640</v>
+      </c>
+      <c r="D194" s="9">
+        <v>31.68</v>
+      </c>
+      <c r="E194">
+        <v>5.6193868502046201E-4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B195">
+        <v>5.6320433947123908E-4</v>
+      </c>
+      <c r="C195" s="8">
+        <v>660</v>
+      </c>
+      <c r="D195" s="9">
+        <v>30.32</v>
+      </c>
+      <c r="E195">
+        <v>5.6320433947123908E-4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B196">
+        <v>5.6631021710881594E-4</v>
+      </c>
+      <c r="C196" s="8">
+        <v>650</v>
+      </c>
+      <c r="D196" s="9">
+        <v>37.549999999999997</v>
+      </c>
+      <c r="E196">
+        <v>5.6631021710881594E-4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B197">
+        <v>5.6756877286444026E-4</v>
+      </c>
+      <c r="C197" s="8">
+        <v>630</v>
+      </c>
+      <c r="D197" s="9">
+        <v>40.75</v>
+      </c>
+      <c r="E197">
+        <v>5.6756877286444026E-4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B198">
+        <v>5.6974426386877282E-4</v>
+      </c>
+      <c r="C198" s="8">
+        <v>580</v>
+      </c>
+      <c r="D198" s="9">
+        <v>46.71</v>
+      </c>
+      <c r="E198">
+        <v>5.6974426386877282E-4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B199">
+        <v>5.7191529004525646E-4</v>
+      </c>
+      <c r="C199" s="8">
+        <v>570</v>
+      </c>
+      <c r="D199" s="9">
+        <v>48.76</v>
+      </c>
+      <c r="E199">
+        <v>5.7191529004525646E-4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B200">
+        <v>5.7316422857142863E-4</v>
+      </c>
+      <c r="C200" s="8">
+        <v>610</v>
+      </c>
+      <c r="D200" s="9">
+        <v>44.65</v>
+      </c>
+      <c r="E200">
+        <v>5.7316422857142863E-4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B201">
+        <v>5.7624400110810759E-4</v>
+      </c>
+      <c r="C201" s="8">
+        <v>600</v>
+      </c>
+      <c r="D201" s="9">
+        <v>44.72</v>
+      </c>
+      <c r="E201">
+        <v>5.7624400110810759E-4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B202">
+        <v>5.7748595526818962E-4</v>
+      </c>
+      <c r="C202" s="8">
+        <v>580</v>
+      </c>
+      <c r="D202" s="9">
+        <v>45.18</v>
+      </c>
+      <c r="E202">
+        <v>5.7748595526818962E-4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B203">
+        <v>5.7872537070857699E-4</v>
+      </c>
+      <c r="C203" s="8">
+        <v>620</v>
+      </c>
+      <c r="D203" s="9">
+        <v>49.78</v>
+      </c>
+      <c r="E203">
+        <v>5.7872537070857699E-4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B204">
+        <v>5.81790031634976E-4</v>
+      </c>
+      <c r="C204" s="8">
+        <v>630</v>
+      </c>
+      <c r="D204" s="9">
+        <v>45.66</v>
+      </c>
+      <c r="E204">
+        <v>5.81790031634976E-4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B205">
+        <v>5.8302252863472951E-4</v>
+      </c>
+      <c r="C205" s="8">
+        <v>690</v>
+      </c>
+      <c r="D205" s="9">
+        <v>51.97</v>
+      </c>
+      <c r="E205">
+        <v>5.8302252863472951E-4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="D206" s="9">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="D207" s="9">
+        <v>53.47</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="D208" s="9">
+        <v>49.33</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4">
+      <c r="D209" s="9">
+        <v>51.06</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4">
+      <c r="D210" s="9">
+        <v>48.48</v>
+      </c>
+    </row>
+    <row r="211" spans="4:4">
+      <c r="D211" s="9">
+        <v>45.18</v>
+      </c>
+    </row>
+    <row r="212" spans="4:4">
+      <c r="D212" s="9">
+        <v>46.63</v>
+      </c>
+    </row>
+    <row r="213" spans="4:4">
+      <c r="D213" s="9">
+        <v>48.04</v>
+      </c>
+    </row>
+    <row r="214" spans="4:4">
+      <c r="D214" s="9">
+        <v>49.82</v>
+      </c>
+    </row>
+    <row r="215" spans="4:4">
+      <c r="D215" s="9">
+        <v>51.58</v>
+      </c>
+    </row>
+    <row r="216" spans="4:4">
+      <c r="D216" s="9">
+        <v>56.64</v>
+      </c>
+    </row>
+    <row r="217" spans="4:4">
+      <c r="D217" s="9">
+        <v>57.88</v>
+      </c>
+    </row>
+    <row r="218" spans="4:4">
+      <c r="D218" s="9">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="219" spans="4:4">
+      <c r="D219" s="9">
+        <v>62.23</v>
+      </c>
+    </row>
+    <row r="220" spans="4:4">
+      <c r="D220" s="9">
+        <v>62.73</v>
+      </c>
+    </row>
+    <row r="221" spans="4:4">
+      <c r="D221" s="9">
+        <v>66.25</v>
+      </c>
+    </row>
+    <row r="222" spans="4:4">
+      <c r="D222" s="9">
+        <v>69.98</v>
+      </c>
+    </row>
+    <row r="223" spans="4:4">
+      <c r="D223" s="9">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="224" spans="4:4">
+      <c r="D224" s="9">
+        <v>70.98</v>
+      </c>
+    </row>
+    <row r="225" spans="4:4">
+      <c r="D225" s="9">
+        <v>68.06</v>
+      </c>
+    </row>
+    <row r="226" spans="4:4">
+      <c r="D226" s="9">
+        <v>70.23</v>
+      </c>
+    </row>
+    <row r="227" spans="4:4">
+      <c r="D227" s="9">
+        <v>70.75</v>
+      </c>
+    </row>
+    <row r="228" spans="4:4">
+      <c r="D228" s="9">
+        <v>56.96</v>
+      </c>
+    </row>
+    <row r="229" spans="4:4">
+      <c r="D229" s="9">
+        <v>49.52</v>
+      </c>
+    </row>
+    <row r="230" spans="4:4">
+      <c r="D230" s="9">
+        <v>51.38</v>
+      </c>
+    </row>
+    <row r="231" spans="4:4">
+      <c r="D231" s="9">
+        <v>54.95</v>
+      </c>
+    </row>
+    <row r="232" spans="4:4">
+      <c r="D232" s="9">
+        <v>58.15</v>
+      </c>
+    </row>
+    <row r="233" spans="4:4">
+      <c r="D233" s="9">
+        <v>63.86</v>
+      </c>
+    </row>
+    <row r="234" spans="4:4">
+      <c r="D234" s="9">
+        <v>60.83</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662F7486-4381-4145-94DB-14583D06F1D7}">
   <dimension ref="A1:R214"/>
   <sheetViews>
@@ -32435,7 +34879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED6B15A-83EF-D046-9845-170FBB6FCCFF}">
   <dimension ref="A1:R214"/>
   <sheetViews>

</xml_diff>

<commit_message>
before change the demand data
</commit_message>
<xml_diff>
--- a/data/correlation/ship_demand_month.xlsx
+++ b/data/correlation/ship_demand_month.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC26DD45-EE67-5148-9781-D32527FEA0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B06C727-BDD1-A14F-800C-6BDD40AA433A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{ABF14036-30F7-DB4A-9800-17033DE06889}"/>
   </bookViews>
   <sheets>
     <sheet name="海事センター" sheetId="5" r:id="rId1"/>
@@ -1096,7 +1096,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>6.9188410682729498E-4</c:v>
+                  <c:v>6.9188410682729487E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.8820870551067283E-4</c:v>
@@ -1240,7 +1240,7 @@
                   <c:v>5.9452975396431654E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5.9032653962288247E-4</c:v>
+                  <c:v>5.9032653962288431E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>5.8618233993985294E-4</c:v>
@@ -13040,8 +13040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40FD581-74FB-F94A-9780-764D633DA0D6}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F210" sqref="F210"/>
+    <sheetView topLeftCell="A121" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G134" sqref="G134:G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -13966,6 +13966,10 @@
       <c r="B37">
         <v>5.8532241516666668</v>
       </c>
+      <c r="C37">
+        <f>SUM(B26:B37)</f>
+        <v>68.072916110833333</v>
+      </c>
       <c r="G37">
         <f t="shared" si="0"/>
         <v>0.61791445607038809</v>
@@ -15739,7 +15743,7 @@
         <v>40179</v>
       </c>
       <c r="B122">
-        <v>9.1837837166666656</v>
+        <v>9.1837837166666692</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -15750,7 +15754,7 @@
       </c>
       <c r="F122">
         <f t="shared" si="2"/>
-        <v>7.0459308611981332E-4</v>
+        <v>7.0459308611981353E-4</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -15970,7 +15974,7 @@
         <v>40544</v>
       </c>
       <c r="B134">
-        <v>9.8207759833333323</v>
+        <v>9.8207759833333306</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -15981,7 +15985,7 @@
       </c>
       <c r="F134">
         <f t="shared" si="9"/>
-        <v>6.9188410682729498E-4</v>
+        <v>6.9188410682729487E-4</v>
       </c>
       <c r="G134">
         <v>1660</v>
@@ -17038,7 +17042,7 @@
         <v>42005</v>
       </c>
       <c r="B182">
-        <v>10.785364266666667</v>
+        <v>10.785364266666701</v>
       </c>
       <c r="D182">
         <v>1</v>
@@ -17049,7 +17053,7 @@
       </c>
       <c r="F182">
         <f t="shared" si="9"/>
-        <v>5.9032653962288247E-4</v>
+        <v>5.9032653962288431E-4</v>
       </c>
       <c r="G182">
         <v>1440</v>
@@ -17646,7 +17650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7311AD3-701D-CE48-8EB0-A330C275BCB3}">
   <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
       <selection activeCell="F208" sqref="F208"/>
     </sheetView>
   </sheetViews>
@@ -24143,7 +24147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE618EF-1A9C-E843-879C-1D2485D28D0D}">
   <dimension ref="A1:S205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G134" sqref="G134:G205"/>
     </sheetView>
   </sheetViews>

</xml_diff>